<commit_message>
Atualização de bases das ligas, do dia: 23-04-2024 às 20:52
</commit_message>
<xml_diff>
--- a/Azerbaijan Premier League/Azerbaijan Premier League.xlsx
+++ b/Azerbaijan Premier League/Azerbaijan Premier League.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -498,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB154"/>
+  <dimension ref="A1:AB155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -661,10 +661,10 @@
         <v>0.95</v>
       </c>
       <c r="Y2">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z2">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -747,10 +747,10 @@
         <v>2.2</v>
       </c>
       <c r="Y3">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z3">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA3">
         <v>0.8999999999999999</v>
@@ -833,10 +833,10 @@
         <v>5</v>
       </c>
       <c r="Y4">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z4">
-        <v>0.45</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA4">
         <v>-1</v>
@@ -919,10 +919,10 @@
         <v>-1</v>
       </c>
       <c r="Y5">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="Z5">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AA5">
         <v>-1</v>
@@ -1005,10 +1005,10 @@
         <v>-1</v>
       </c>
       <c r="Y6">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="Z6">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA6">
         <v>0.825</v>
@@ -1091,10 +1091,10 @@
         <v>-1</v>
       </c>
       <c r="Y7">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z7">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA7">
         <v>-0.5</v>
@@ -1177,10 +1177,10 @@
         <v>-1</v>
       </c>
       <c r="Y8">
-        <v>-1</v>
+        <v>0.3875</v>
       </c>
       <c r="Z8">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AA8">
         <v>-1</v>
@@ -1263,10 +1263,10 @@
         <v>-1</v>
       </c>
       <c r="Y9">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z9">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA9">
         <v>0.4125</v>
@@ -1435,10 +1435,10 @@
         <v>1.7</v>
       </c>
       <c r="Y11">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="Z11">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA11">
         <v>-0.5</v>
@@ -1521,10 +1521,10 @@
         <v>2.6</v>
       </c>
       <c r="Y12">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z12">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA12">
         <v>0.925</v>
@@ -1607,10 +1607,10 @@
         <v>1.2</v>
       </c>
       <c r="Y13">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="Z13">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA13">
         <v>0.8</v>
@@ -1951,10 +1951,10 @@
         <v>2.5</v>
       </c>
       <c r="Y17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z17">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA17">
         <v>0.8</v>
@@ -2037,10 +2037,10 @@
         <v>-1</v>
       </c>
       <c r="Y18">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z18">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA18">
         <v>-1</v>
@@ -2123,10 +2123,10 @@
         <v>-1</v>
       </c>
       <c r="Y19">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z19">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA19">
         <v>-1</v>
@@ -2295,10 +2295,10 @@
         <v>7.5</v>
       </c>
       <c r="Y21">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z21">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA21">
         <v>0.475</v>
@@ -2381,10 +2381,10 @@
         <v>-1</v>
       </c>
       <c r="Y22">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z22">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA22">
         <v>-1</v>
@@ -2467,10 +2467,10 @@
         <v>0.571</v>
       </c>
       <c r="Y23">
-        <v>0.7749999999999999</v>
+        <v>0</v>
       </c>
       <c r="Z23">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA23">
         <v>-1</v>
@@ -2553,10 +2553,10 @@
         <v>1.625</v>
       </c>
       <c r="Y24">
+        <v>-1</v>
+      </c>
+      <c r="Z24">
         <v>0.8999999999999999</v>
-      </c>
-      <c r="Z24">
-        <v>-1</v>
       </c>
       <c r="AA24">
         <v>1.025</v>
@@ -2725,10 +2725,10 @@
         <v>-1</v>
       </c>
       <c r="Y26">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="Z26">
-        <v>0.8500000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AA26">
         <v>-1</v>
@@ -2811,10 +2811,10 @@
         <v>1.6</v>
       </c>
       <c r="Y27">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="Z27">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA27">
         <v>1.025</v>
@@ -2897,10 +2897,10 @@
         <v>-1</v>
       </c>
       <c r="Y28">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z28">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA28">
         <v>-1</v>
@@ -3069,10 +3069,10 @@
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z30">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA30">
         <v>-1</v>
@@ -3327,10 +3327,10 @@
         <v>-1</v>
       </c>
       <c r="Y33">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z33">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA33">
         <v>-1</v>
@@ -3499,10 +3499,10 @@
         <v>-1</v>
       </c>
       <c r="Y35">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z35">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA35">
         <v>0.8</v>
@@ -3585,10 +3585,10 @@
         <v>1.05</v>
       </c>
       <c r="Y36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z36">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA36">
         <v>-1</v>
@@ -3757,10 +3757,10 @@
         <v>1.25</v>
       </c>
       <c r="Y38">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z38">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA38">
         <v>-1</v>
@@ -3843,10 +3843,10 @@
         <v>-1</v>
       </c>
       <c r="Y39">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z39">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA39">
         <v>-1</v>
@@ -3929,10 +3929,10 @@
         <v>-1</v>
       </c>
       <c r="Y40">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z40">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA40">
         <v>1</v>
@@ -4015,10 +4015,10 @@
         <v>2.2</v>
       </c>
       <c r="Y41">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="Z41">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA41">
         <v>-1</v>
@@ -4187,10 +4187,10 @@
         <v>-1</v>
       </c>
       <c r="Y43">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z43">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA43">
         <v>-1</v>
@@ -4273,10 +4273,10 @@
         <v>0.7270000000000001</v>
       </c>
       <c r="Y44">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z44">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA44">
         <v>-1</v>
@@ -4445,10 +4445,10 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="Y46">
+        <v>-1</v>
+      </c>
+      <c r="Z46">
         <v>0.8999999999999999</v>
-      </c>
-      <c r="Z46">
-        <v>-1</v>
       </c>
       <c r="AA46">
         <v>1</v>
@@ -4617,10 +4617,10 @@
         <v>-1</v>
       </c>
       <c r="Y48">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z48">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA48">
         <v>0.875</v>
@@ -4703,10 +4703,10 @@
         <v>2.1</v>
       </c>
       <c r="Y49">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z49">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA49">
         <v>0.95</v>
@@ -4789,10 +4789,10 @@
         <v>-1</v>
       </c>
       <c r="Y50">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z50">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA50">
         <v>-1</v>
@@ -4961,10 +4961,10 @@
         <v>-1</v>
       </c>
       <c r="Y52">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="Z52">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA52">
         <v>0.9750000000000001</v>
@@ -5133,10 +5133,10 @@
         <v>1.45</v>
       </c>
       <c r="Y54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z54">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA54">
         <v>-1</v>
@@ -5219,10 +5219,10 @@
         <v>-1</v>
       </c>
       <c r="Y55">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA55">
         <v>0.4875</v>
@@ -5305,10 +5305,10 @@
         <v>-1</v>
       </c>
       <c r="Y56">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z56">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA56">
         <v>0.925</v>
@@ -5391,10 +5391,10 @@
         <v>-1</v>
       </c>
       <c r="Y57">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z57">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA57">
         <v>0.925</v>
@@ -5477,10 +5477,10 @@
         <v>-1</v>
       </c>
       <c r="Y58">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="Z58">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA58">
         <v>0</v>
@@ -5563,10 +5563,10 @@
         <v>1.15</v>
       </c>
       <c r="Y59">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z59">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA59">
         <v>-0.5</v>
@@ -5649,10 +5649,10 @@
         <v>2.75</v>
       </c>
       <c r="Y60">
+        <v>-1</v>
+      </c>
+      <c r="Z60">
         <v>0.8999999999999999</v>
-      </c>
-      <c r="Z60">
-        <v>-1</v>
       </c>
       <c r="AA60">
         <v>-1</v>
@@ -5735,10 +5735,10 @@
         <v>4.5</v>
       </c>
       <c r="Y61">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z61">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA61">
         <v>-1</v>
@@ -5821,10 +5821,10 @@
         <v>4</v>
       </c>
       <c r="Y62">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z62">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA62">
         <v>0.825</v>
@@ -5907,10 +5907,10 @@
         <v>0.909</v>
       </c>
       <c r="Y63">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z63">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA63">
         <v>1</v>
@@ -5993,10 +5993,10 @@
         <v>-1</v>
       </c>
       <c r="Y64">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z64">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA64">
         <v>-1</v>
@@ -6079,10 +6079,10 @@
         <v>-1</v>
       </c>
       <c r="Y65">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z65">
-        <v>0.875</v>
+        <v>0.4375</v>
       </c>
       <c r="AA65">
         <v>0.925</v>
@@ -6165,10 +6165,10 @@
         <v>0.7</v>
       </c>
       <c r="Y66">
-        <v>0.8500000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="Z66">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AA66">
         <v>0.4625</v>
@@ -6337,10 +6337,10 @@
         <v>-1</v>
       </c>
       <c r="Y68">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="Z68">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA68">
         <v>0.8500000000000001</v>
@@ -6767,10 +6767,10 @@
         <v>0.55</v>
       </c>
       <c r="Y73">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA73">
         <v>-0.5</v>
@@ -6853,10 +6853,10 @@
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z74">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
         <v>-1</v>
@@ -6939,10 +6939,10 @@
         <v>-1</v>
       </c>
       <c r="Y75">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z75">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA75">
         <v>0.4125</v>
@@ -7025,10 +7025,10 @@
         <v>0.363</v>
       </c>
       <c r="Y76">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="Z76">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA76">
         <v>0.925</v>
@@ -7111,10 +7111,10 @@
         <v>3.2</v>
       </c>
       <c r="Y77">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="Z77">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA77">
         <v>0.825</v>
@@ -7283,10 +7283,10 @@
         <v>-1</v>
       </c>
       <c r="Y79">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z79">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA79">
         <v>0.8999999999999999</v>
@@ -7369,10 +7369,10 @@
         <v>-1</v>
       </c>
       <c r="Y80">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="Z80">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA80">
         <v>0.8</v>
@@ -7541,10 +7541,10 @@
         <v>-1</v>
       </c>
       <c r="Y82">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z82">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA82">
         <v>0.95</v>
@@ -7627,10 +7627,10 @@
         <v>-1</v>
       </c>
       <c r="Y83">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z83">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA83">
         <v>-1</v>
@@ -7713,10 +7713,10 @@
         <v>-1</v>
       </c>
       <c r="Y84">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z84">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA84">
         <v>-1</v>
@@ -7799,10 +7799,10 @@
         <v>-1</v>
       </c>
       <c r="Y85">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z85">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA85">
         <v>-1</v>
@@ -7885,10 +7885,10 @@
         <v>-1</v>
       </c>
       <c r="Y86">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="Z86">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AA86">
         <v>-1</v>
@@ -7971,10 +7971,10 @@
         <v>-1</v>
       </c>
       <c r="Y87">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z87">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA87">
         <v>-1</v>
@@ -8057,10 +8057,10 @@
         <v>-1</v>
       </c>
       <c r="Y88">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="Z88">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA88">
         <v>0.95</v>
@@ -8143,10 +8143,10 @@
         <v>-1</v>
       </c>
       <c r="Y89">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="Z89">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA89">
         <v>-1</v>
@@ -8229,10 +8229,10 @@
         <v>0.444</v>
       </c>
       <c r="Y90">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="Z90">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AA90">
         <v>-1</v>
@@ -8487,10 +8487,10 @@
         <v>-1</v>
       </c>
       <c r="Y93">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="Z93">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA93">
         <v>0.825</v>
@@ -8573,10 +8573,10 @@
         <v>1.55</v>
       </c>
       <c r="Y94">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="Z94">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA94">
         <v>-1</v>
@@ -8659,10 +8659,10 @@
         <v>-1</v>
       </c>
       <c r="Y95">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="Z95">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="AA95">
         <v>0.95</v>
@@ -8745,10 +8745,10 @@
         <v>-1</v>
       </c>
       <c r="Y96">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z96">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA96">
         <v>0.7250000000000001</v>
@@ -8917,10 +8917,10 @@
         <v>1.2</v>
       </c>
       <c r="Y98">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z98">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA98">
         <v>-1</v>
@@ -9089,10 +9089,10 @@
         <v>-1</v>
       </c>
       <c r="Y100">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z100">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA100">
         <v>0.95</v>
@@ -9347,10 +9347,10 @@
         <v>-1</v>
       </c>
       <c r="Y103">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z103">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA103">
         <v>0.8500000000000001</v>
@@ -9519,10 +9519,10 @@
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z105">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
         <v>0.95</v>
@@ -9691,10 +9691,10 @@
         <v>2</v>
       </c>
       <c r="Y107">
+        <v>-1</v>
+      </c>
+      <c r="Z107">
         <v>0.8999999999999999</v>
-      </c>
-      <c r="Z107">
-        <v>-1</v>
       </c>
       <c r="AA107">
         <v>0.95</v>
@@ -9777,10 +9777,10 @@
         <v>-1</v>
       </c>
       <c r="Y108">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="Z108">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AA108">
         <v>0.7749999999999999</v>
@@ -9949,10 +9949,10 @@
         <v>-1</v>
       </c>
       <c r="Y110">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z110">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA110">
         <v>-1</v>
@@ -10035,10 +10035,10 @@
         <v>-1</v>
       </c>
       <c r="Y111">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Z111">
-        <v>0.8999999999999999</v>
+        <v>-0.5</v>
       </c>
       <c r="AA111">
         <v>0.875</v>
@@ -10293,10 +10293,10 @@
         <v>-1</v>
       </c>
       <c r="Y114">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z114">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA114">
         <v>-1</v>
@@ -10379,10 +10379,10 @@
         <v>-1</v>
       </c>
       <c r="Y115">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z115">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA115">
         <v>0.825</v>
@@ -10551,10 +10551,10 @@
         <v>-1</v>
       </c>
       <c r="Y117">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z117">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA117">
         <v>-1</v>
@@ -10637,10 +10637,10 @@
         <v>1.9</v>
       </c>
       <c r="Y118">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="Z118">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA118">
         <v>0.8</v>
@@ -10723,10 +10723,10 @@
         <v>-1</v>
       </c>
       <c r="Y119">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z119">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA119">
         <v>-1</v>
@@ -10809,10 +10809,10 @@
         <v>0.2849999999999999</v>
       </c>
       <c r="Y120">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="Z120">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA120">
         <v>0.9750000000000001</v>
@@ -10895,10 +10895,10 @@
         <v>2.4</v>
       </c>
       <c r="Y121">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z121">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA121">
         <v>0.925</v>
@@ -11067,10 +11067,10 @@
         <v>-1</v>
       </c>
       <c r="Y123">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z123">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA123">
         <v>-0.5</v>
@@ -11153,10 +11153,10 @@
         <v>1</v>
       </c>
       <c r="Y124">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z124">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA124">
         <v>0.95</v>
@@ -11239,10 +11239,10 @@
         <v>0.7</v>
       </c>
       <c r="Y125">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="Z125">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA125">
         <v>0.825</v>
@@ -11325,10 +11325,10 @@
         <v>2</v>
       </c>
       <c r="Y126">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="Z126">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA126">
         <v>-1</v>
@@ -11497,10 +11497,10 @@
         <v>-1</v>
       </c>
       <c r="Y128">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z128">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="AA128">
         <v>0.825</v>
@@ -11583,10 +11583,10 @@
         <v>-1</v>
       </c>
       <c r="Y129">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z129">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA129">
         <v>-0.5</v>
@@ -11669,10 +11669,10 @@
         <v>-1</v>
       </c>
       <c r="Y130">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z130">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA130">
         <v>1</v>
@@ -11755,10 +11755,10 @@
         <v>-1</v>
       </c>
       <c r="Y131">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z131">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA131">
         <v>0.7749999999999999</v>
@@ -11841,10 +11841,10 @@
         <v>-1</v>
       </c>
       <c r="Y132">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="Z132">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AA132">
         <v>0.9750000000000001</v>
@@ -12013,10 +12013,10 @@
         <v>0.55</v>
       </c>
       <c r="Y134">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="Z134">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA134">
         <v>0.875</v>
@@ -12099,10 +12099,10 @@
         <v>1.15</v>
       </c>
       <c r="Y135">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z135">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA135">
         <v>0.95</v>
@@ -12185,10 +12185,10 @@
         <v>0.95</v>
       </c>
       <c r="Y136">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="Z136">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA136">
         <v>-1</v>
@@ -12271,10 +12271,10 @@
         <v>0.25</v>
       </c>
       <c r="Y137">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z137">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA137">
         <v>0.8500000000000001</v>
@@ -12443,10 +12443,10 @@
         <v>2.5</v>
       </c>
       <c r="Y139">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z139">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA139">
         <v>-1</v>
@@ -12529,10 +12529,10 @@
         <v>-1</v>
       </c>
       <c r="Y140">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z140">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA140">
         <v>-1</v>
@@ -12615,10 +12615,10 @@
         <v>2.2</v>
       </c>
       <c r="Y141">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z141">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA141">
         <v>0.8</v>
@@ -12701,10 +12701,10 @@
         <v>-1</v>
       </c>
       <c r="Y142">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z142">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA142">
         <v>-0.5</v>
@@ -12787,10 +12787,10 @@
         <v>-1</v>
       </c>
       <c r="Y143">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z143">
-        <v>0.8500000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="AA143">
         <v>0.9750000000000001</v>
@@ -12873,10 +12873,10 @@
         <v>-1</v>
       </c>
       <c r="Y144">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="Z144">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA144">
         <v>0.8999999999999999</v>
@@ -13131,10 +13131,10 @@
         <v>1.15</v>
       </c>
       <c r="Y147">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z147">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA147">
         <v>0.75</v>
@@ -13217,10 +13217,10 @@
         <v>-1</v>
       </c>
       <c r="Y148">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="Z148">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA148">
         <v>0.8</v>
@@ -13389,10 +13389,10 @@
         <v>-1</v>
       </c>
       <c r="Y150">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z150">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
       <c r="AA150">
         <v>0.8500000000000001</v>
@@ -13475,10 +13475,10 @@
         <v>2.4</v>
       </c>
       <c r="Y151">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z151">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA151">
         <v>1.025</v>
@@ -13647,10 +13647,10 @@
         <v>-1</v>
       </c>
       <c r="Y153">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z153">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA153">
         <v>0.7250000000000001</v>
@@ -13733,16 +13733,102 @@
         <v>0.75</v>
       </c>
       <c r="Y154">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Z154">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AA154">
         <v>0.4</v>
       </c>
       <c r="AB154">
         <v>-0.5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:28">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>7020806</v>
+      </c>
+      <c r="C155" t="s">
+        <v>27</v>
+      </c>
+      <c r="D155" s="2">
+        <v>45403.5</v>
+      </c>
+      <c r="E155" t="s">
+        <v>28</v>
+      </c>
+      <c r="F155" t="s">
+        <v>29</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>2</v>
+      </c>
+      <c r="I155" t="s">
+        <v>38</v>
+      </c>
+      <c r="J155">
+        <v>2.5</v>
+      </c>
+      <c r="K155">
+        <v>3.2</v>
+      </c>
+      <c r="L155">
+        <v>2.5</v>
+      </c>
+      <c r="M155">
+        <v>2.2</v>
+      </c>
+      <c r="N155">
+        <v>3.2</v>
+      </c>
+      <c r="O155">
+        <v>2.9</v>
+      </c>
+      <c r="P155">
+        <v>-0.25</v>
+      </c>
+      <c r="Q155">
+        <v>2</v>
+      </c>
+      <c r="R155">
+        <v>1.8</v>
+      </c>
+      <c r="S155">
+        <v>2.5</v>
+      </c>
+      <c r="T155">
+        <v>1.925</v>
+      </c>
+      <c r="U155">
+        <v>1.875</v>
+      </c>
+      <c r="V155">
+        <v>-1</v>
+      </c>
+      <c r="W155">
+        <v>-1</v>
+      </c>
+      <c r="X155">
+        <v>1.9</v>
+      </c>
+      <c r="Y155">
+        <v>-1</v>
+      </c>
+      <c r="Z155">
+        <v>0.8</v>
+      </c>
+      <c r="AA155">
+        <v>-1</v>
+      </c>
+      <c r="AB155">
+        <v>0.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 27-04-2024 às 09:20
</commit_message>
<xml_diff>
--- a/Azerbaijan Premier League/Azerbaijan Premier League.xlsx
+++ b/Azerbaijan Premier League/Azerbaijan Premier League.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>PL_AhUnder</t>
+  </si>
+  <si>
+    <t>7071263</t>
   </si>
   <si>
     <t>Azerbaijan Premier League</t>
@@ -498,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB155"/>
+  <dimension ref="A1:AB156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -595,16 +598,16 @@
         <v>6943460</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2">
         <v>45142.54166666666</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -613,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2">
         <v>2.1</v>
@@ -681,16 +684,16 @@
         <v>6943462</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2">
         <v>45143.47916666666</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -699,7 +702,7 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -767,16 +770,16 @@
         <v>6942350</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2">
         <v>45143.58333333334</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -785,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J4">
         <v>1.181</v>
@@ -853,16 +856,16 @@
         <v>6943461</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2">
         <v>45144.41666666666</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -871,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -939,16 +942,16 @@
         <v>6940298</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2">
         <v>45144.54166666666</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -957,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J6">
         <v>1.571</v>
@@ -1025,16 +1028,16 @@
         <v>6943463</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2">
         <v>45150.47916666666</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1043,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -1111,16 +1114,16 @@
         <v>6943465</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2">
         <v>45150.58333333334</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1129,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J8">
         <v>1.571</v>
@@ -1197,16 +1200,16 @@
         <v>6942351</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2">
         <v>45151.47916666666</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -1215,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J9">
         <v>1.533</v>
@@ -1283,16 +1286,16 @@
         <v>6943464</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2">
         <v>45152.54166666666</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1301,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J10">
         <v>1.5</v>
@@ -1369,16 +1372,16 @@
         <v>6943466</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>45156.41666666666</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1387,7 +1390,7 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J11">
         <v>2.3</v>
@@ -1455,16 +1458,16 @@
         <v>6943468</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2">
         <v>45157.45833333334</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1473,7 +1476,7 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J12">
         <v>2.1</v>
@@ -1541,16 +1544,16 @@
         <v>6943467</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2">
         <v>45157.54166666666</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1559,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J13">
         <v>3.5</v>
@@ -1627,16 +1630,16 @@
         <v>6944562</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2">
         <v>45158.45833333334</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1645,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J14">
         <v>1.166</v>
@@ -1713,16 +1716,16 @@
         <v>6940300</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2">
         <v>45158.54166666666</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1731,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J15">
         <v>1.5</v>
@@ -1799,16 +1802,16 @@
         <v>6943469</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2">
         <v>45163.54166666666</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1817,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J16">
         <v>2.4</v>
@@ -1885,16 +1888,16 @@
         <v>6943471</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2">
         <v>45164.41666666666</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1903,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J17">
         <v>2.4</v>
@@ -1971,16 +1974,16 @@
         <v>6940301</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2">
         <v>45164.52083333334</v>
       </c>
       <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
         <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1989,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J18">
         <v>3.1</v>
@@ -2057,16 +2060,16 @@
         <v>6943470</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2">
         <v>45165.47916666666</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -2075,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J19">
         <v>1.833</v>
@@ -2143,16 +2146,16 @@
         <v>6942352</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2">
         <v>45165.57291666666</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2161,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J20">
         <v>1.166</v>
@@ -2229,16 +2232,16 @@
         <v>6940302</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2">
         <v>45170.5</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2247,7 +2250,7 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J21">
         <v>1.444</v>
@@ -2315,16 +2318,16 @@
         <v>6943473</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
         <v>45171.45833333334</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2333,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J22">
         <v>4.333</v>
@@ -2401,16 +2404,16 @@
         <v>6943474</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2">
         <v>45171.5625</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2419,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J23">
         <v>4.75</v>
@@ -2487,16 +2490,16 @@
         <v>6943472</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="2">
         <v>45172.41666666666</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2505,7 +2508,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J24">
         <v>2.375</v>
@@ -2573,16 +2576,16 @@
         <v>6942353</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2">
         <v>45172.52083333334</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -2591,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J25">
         <v>9</v>
@@ -2659,16 +2662,16 @@
         <v>6976494</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2">
         <v>45184.41666666666</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2677,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J26">
         <v>1.6</v>
@@ -2745,16 +2748,16 @@
         <v>6976497</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D27" s="2">
         <v>45185.375</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2763,7 +2766,7 @@
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J27">
         <v>2.5</v>
@@ -2831,16 +2834,16 @@
         <v>6976493</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2">
         <v>45185.45833333334</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2849,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J28">
         <v>5</v>
@@ -2917,17 +2920,17 @@
         <v>6976495</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2">
         <v>45186.39583333334</v>
       </c>
       <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
         <v>36</v>
       </c>
-      <c r="F29" t="s">
-        <v>35</v>
-      </c>
       <c r="G29">
         <v>2</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J29">
         <v>2.5</v>
@@ -3003,16 +3006,16 @@
         <v>6976496</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D30" s="2">
         <v>45186.52083333334</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -3021,7 +3024,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J30">
         <v>1.533</v>
@@ -3089,17 +3092,17 @@
         <v>6976500</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D31" s="2">
         <v>45192.45833333334</v>
       </c>
       <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" t="s">
         <v>37</v>
       </c>
-      <c r="F31" t="s">
-        <v>36</v>
-      </c>
       <c r="G31">
         <v>0</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J31">
         <v>2.55</v>
@@ -3175,17 +3178,17 @@
         <v>6977259</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D32" s="2">
         <v>45193.41666666666</v>
       </c>
       <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" t="s">
         <v>32</v>
       </c>
-      <c r="F32" t="s">
-        <v>31</v>
-      </c>
       <c r="G32">
         <v>2</v>
       </c>
@@ -3193,7 +3196,7 @@
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J32">
         <v>1.533</v>
@@ -3261,16 +3264,16 @@
         <v>6976498</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D33" s="2">
         <v>45193.52083333334</v>
       </c>
       <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
         <v>29</v>
-      </c>
-      <c r="F33" t="s">
-        <v>28</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -3279,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J33">
         <v>2.3</v>
@@ -3347,16 +3350,16 @@
         <v>6976499</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D34" s="2">
         <v>45194.5</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -3365,7 +3368,7 @@
         <v>2</v>
       </c>
       <c r="I34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J34">
         <v>6.5</v>
@@ -3433,16 +3436,16 @@
         <v>6976504</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D35" s="2">
         <v>45198.54166666666</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G35">
         <v>5</v>
@@ -3451,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J35">
         <v>1.285</v>
@@ -3519,16 +3522,16 @@
         <v>6976503</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D36" s="2">
         <v>45199.375</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -3537,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J36">
         <v>2.5</v>
@@ -3605,16 +3608,16 @@
         <v>6976506</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D37" s="2">
         <v>45199.45833333334</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G37">
         <v>2</v>
@@ -3623,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J37">
         <v>2.8</v>
@@ -3691,16 +3694,16 @@
         <v>6976505</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D38" s="2">
         <v>45200.375</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3709,7 +3712,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J38">
         <v>2.375</v>
@@ -3777,16 +3780,16 @@
         <v>6976502</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D39" s="2">
         <v>45200.47916666666</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -3795,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J39">
         <v>2.5</v>
@@ -3863,16 +3866,16 @@
         <v>7011536</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D40" s="2">
         <v>45205.45833333334</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F40" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G40">
         <v>2</v>
@@ -3881,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J40">
         <v>1.5</v>
@@ -3949,16 +3952,16 @@
         <v>7011533</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D41" s="2">
         <v>45206.375</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -3967,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J41">
         <v>2.25</v>
@@ -4035,16 +4038,16 @@
         <v>7011532</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D42" s="2">
         <v>45206.45833333334</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -4053,7 +4056,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J42">
         <v>1.8</v>
@@ -4121,16 +4124,16 @@
         <v>7011534</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D43" s="2">
         <v>45207.39583333334</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -4139,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J43">
         <v>2.25</v>
@@ -4207,16 +4210,16 @@
         <v>7011535</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D44" s="2">
         <v>45207.52083333334</v>
       </c>
       <c r="E44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F44" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -4225,7 +4228,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J44">
         <v>4.8</v>
@@ -4293,16 +4296,16 @@
         <v>7011541</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D45" s="2">
         <v>45219.47916666666</v>
       </c>
       <c r="E45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F45" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G45">
         <v>2</v>
@@ -4311,7 +4314,7 @@
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J45">
         <v>7</v>
@@ -4379,16 +4382,16 @@
         <v>7011539</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D46" s="2">
         <v>45219.5625</v>
       </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -4397,7 +4400,7 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J46">
         <v>3</v>
@@ -4465,16 +4468,16 @@
         <v>7011540</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D47" s="2">
         <v>45220.33333333334</v>
       </c>
       <c r="E47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -4483,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J47">
         <v>5.5</v>
@@ -4551,16 +4554,16 @@
         <v>7011538</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D48" s="2">
         <v>45220.45833333334</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G48">
         <v>3</v>
@@ -4569,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J48">
         <v>1.75</v>
@@ -4637,16 +4640,16 @@
         <v>7011537</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D49" s="2">
         <v>45221.39583333334</v>
       </c>
       <c r="E49" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -4655,7 +4658,7 @@
         <v>4</v>
       </c>
       <c r="I49" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J49">
         <v>2</v>
@@ -4723,16 +4726,16 @@
         <v>7267423</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D50" s="2">
         <v>45224.47916666666</v>
       </c>
       <c r="E50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F50" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -4741,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J50">
         <v>5</v>
@@ -4809,16 +4812,16 @@
         <v>7011544</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D51" s="2">
         <v>45227.375</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G51">
         <v>2</v>
@@ -4827,7 +4830,7 @@
         <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J51">
         <v>2</v>
@@ -4895,16 +4898,16 @@
         <v>7011543</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D52" s="2">
         <v>45227.5</v>
       </c>
       <c r="E52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F52" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G52">
         <v>4</v>
@@ -4913,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J52">
         <v>2.25</v>
@@ -4981,16 +4984,16 @@
         <v>7011546</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D53" s="2">
         <v>45228.375</v>
       </c>
       <c r="E53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F53" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -4999,7 +5002,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J53">
         <v>2.2</v>
@@ -5067,16 +5070,16 @@
         <v>7011545</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D54" s="2">
         <v>45228.47916666666</v>
       </c>
       <c r="E54" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F54" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -5085,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J54">
         <v>2.5</v>
@@ -5153,16 +5156,16 @@
         <v>7011542</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D55" s="2">
         <v>45229.5</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F55" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G55">
         <v>2</v>
@@ -5171,7 +5174,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J55">
         <v>5.75</v>
@@ -5239,16 +5242,16 @@
         <v>7011549</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D56" s="2">
         <v>45233.5</v>
       </c>
       <c r="E56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F56" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -5257,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J56">
         <v>2.25</v>
@@ -5325,16 +5328,16 @@
         <v>7011591</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D57" s="2">
         <v>45234.375</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F57" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G57">
         <v>7</v>
@@ -5343,7 +5346,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J57">
         <v>1.125</v>
@@ -5411,16 +5414,16 @@
         <v>7011547</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D58" s="2">
         <v>45234.45833333334</v>
       </c>
       <c r="E58" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F58" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G58">
         <v>2</v>
@@ -5429,7 +5432,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J58">
         <v>2.75</v>
@@ -5497,17 +5500,17 @@
         <v>7011551</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D59" s="2">
         <v>45235.375</v>
       </c>
       <c r="E59" t="s">
+        <v>36</v>
+      </c>
+      <c r="F59" t="s">
         <v>35</v>
       </c>
-      <c r="F59" t="s">
-        <v>34</v>
-      </c>
       <c r="G59">
         <v>0</v>
       </c>
@@ -5515,7 +5518,7 @@
         <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J59">
         <v>3.6</v>
@@ -5583,16 +5586,16 @@
         <v>7011548</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D60" s="2">
         <v>45235.47916666666</v>
       </c>
       <c r="E60" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F60" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -5601,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J60">
         <v>2.25</v>
@@ -5669,16 +5672,16 @@
         <v>7011552</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D61" s="2">
         <v>45240.5</v>
       </c>
       <c r="E61" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -5687,7 +5690,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J61">
         <v>1.4</v>
@@ -5755,16 +5758,16 @@
         <v>7011556</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D62" s="2">
         <v>45241.39583333334</v>
       </c>
       <c r="E62" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F62" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -5773,7 +5776,7 @@
         <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J62">
         <v>1.5</v>
@@ -5841,16 +5844,16 @@
         <v>7011554</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D63" s="2">
         <v>45241.5</v>
       </c>
       <c r="E63" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F63" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -5859,7 +5862,7 @@
         <v>3</v>
       </c>
       <c r="I63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J63">
         <v>3.1</v>
@@ -5927,16 +5930,16 @@
         <v>7011555</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D64" s="2">
         <v>45242.39583333334</v>
       </c>
       <c r="E64" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F64" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -5945,7 +5948,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J64">
         <v>1.95</v>
@@ -6013,16 +6016,16 @@
         <v>7011553</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D65" s="2">
         <v>45242.5</v>
       </c>
       <c r="E65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" t="s">
         <v>30</v>
-      </c>
-      <c r="F65" t="s">
-        <v>29</v>
       </c>
       <c r="G65">
         <v>3</v>
@@ -6031,7 +6034,7 @@
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J65">
         <v>1.222</v>
@@ -6099,16 +6102,16 @@
         <v>7011560</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D66" s="2">
         <v>45254.54166666666</v>
       </c>
       <c r="E66" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -6117,7 +6120,7 @@
         <v>2</v>
       </c>
       <c r="I66" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J66">
         <v>4</v>
@@ -6185,16 +6188,16 @@
         <v>7011561</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D67" s="2">
         <v>45255.29166666666</v>
       </c>
       <c r="E67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -6203,7 +6206,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J67">
         <v>1.65</v>
@@ -6271,16 +6274,16 @@
         <v>7011559</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D68" s="2">
         <v>45255.375</v>
       </c>
       <c r="E68" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F68" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G68">
         <v>4</v>
@@ -6289,7 +6292,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J68">
         <v>2.2</v>
@@ -6357,16 +6360,16 @@
         <v>7011557</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D69" s="2">
         <v>45256.35416666666</v>
       </c>
       <c r="E69" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F69" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -6375,7 +6378,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J69">
         <v>1.6</v>
@@ -6443,16 +6446,16 @@
         <v>7011558</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D70" s="2">
         <v>45256.45833333334</v>
       </c>
       <c r="E70" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F70" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -6461,7 +6464,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J70">
         <v>3.1</v>
@@ -6529,16 +6532,16 @@
         <v>7011562</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D71" s="2">
         <v>45262.375</v>
       </c>
       <c r="E71" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F71" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -6547,7 +6550,7 @@
         <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J71">
         <v>2.2</v>
@@ -6615,16 +6618,16 @@
         <v>7011565</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D72" s="2">
         <v>45262.47916666666</v>
       </c>
       <c r="E72" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F72" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G72">
         <v>2</v>
@@ -6633,7 +6636,7 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J72">
         <v>2.375</v>
@@ -6701,16 +6704,16 @@
         <v>7011563</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D73" s="2">
         <v>45263.33333333334</v>
       </c>
       <c r="E73" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F73" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -6719,7 +6722,7 @@
         <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J73">
         <v>3.6</v>
@@ -6787,16 +6790,16 @@
         <v>7011566</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D74" s="2">
         <v>45263.41666666666</v>
       </c>
       <c r="E74" t="s">
+        <v>35</v>
+      </c>
+      <c r="F74" t="s">
         <v>34</v>
-      </c>
-      <c r="F74" t="s">
-        <v>33</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -6805,7 +6808,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J74">
         <v>2</v>
@@ -6873,16 +6876,16 @@
         <v>7011564</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D75" s="2">
         <v>45264.52083333334</v>
       </c>
       <c r="E75" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F75" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G75">
         <v>3</v>
@@ -6891,7 +6894,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J75">
         <v>1.181</v>
@@ -6959,16 +6962,16 @@
         <v>7011569</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D76" s="2">
         <v>45268.52083333334</v>
       </c>
       <c r="E76" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F76" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -6977,7 +6980,7 @@
         <v>6</v>
       </c>
       <c r="I76" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J76">
         <v>4.333</v>
@@ -7045,16 +7048,16 @@
         <v>7011570</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D77" s="2">
         <v>45269.33333333334</v>
       </c>
       <c r="E77" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F77" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -7063,7 +7066,7 @@
         <v>3</v>
       </c>
       <c r="I77" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J77">
         <v>1.727</v>
@@ -7131,16 +7134,16 @@
         <v>7011567</v>
       </c>
       <c r="C78" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D78" s="2">
         <v>45269.41666666666</v>
       </c>
       <c r="E78" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F78" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -7149,7 +7152,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J78">
         <v>1.666</v>
@@ -7217,16 +7220,16 @@
         <v>7011571</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D79" s="2">
         <v>45270.33333333334</v>
       </c>
       <c r="E79" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F79" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G79">
         <v>4</v>
@@ -7235,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J79">
         <v>1.615</v>
@@ -7303,16 +7306,16 @@
         <v>7011568</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D80" s="2">
         <v>45270.45833333334</v>
       </c>
       <c r="E80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F80" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G80">
         <v>3</v>
@@ -7321,7 +7324,7 @@
         <v>2</v>
       </c>
       <c r="I80" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J80">
         <v>2</v>
@@ -7389,16 +7392,16 @@
         <v>7011574</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D81" s="2">
         <v>45274.35416666666</v>
       </c>
       <c r="E81" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -7407,7 +7410,7 @@
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J81">
         <v>2.625</v>
@@ -7475,16 +7478,16 @@
         <v>7011573</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D82" s="2">
         <v>45275.25</v>
       </c>
       <c r="E82" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F82" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G82">
         <v>3</v>
@@ -7493,7 +7496,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J82">
         <v>2.1</v>
@@ -7561,16 +7564,16 @@
         <v>7011572</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D83" s="2">
         <v>45275.33333333334</v>
       </c>
       <c r="E83" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F83" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G83">
         <v>2</v>
@@ -7579,7 +7582,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J83">
         <v>2.3</v>
@@ -7647,16 +7650,16 @@
         <v>7011576</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D84" s="2">
         <v>45276.45833333334</v>
       </c>
       <c r="E84" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F84" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -7665,7 +7668,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J84">
         <v>3</v>
@@ -7733,16 +7736,16 @@
         <v>7011575</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D85" s="2">
         <v>45278.54166666666</v>
       </c>
       <c r="E85" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F85" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G85">
         <v>2</v>
@@ -7751,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J85">
         <v>1.363</v>
@@ -7819,16 +7822,16 @@
         <v>7011581</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D86" s="2">
         <v>45282.375</v>
       </c>
       <c r="E86" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F86" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -7837,7 +7840,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J86">
         <v>4</v>
@@ -7905,16 +7908,16 @@
         <v>7011580</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D87" s="2">
         <v>45283.47916666666</v>
       </c>
       <c r="E87" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F87" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -7923,7 +7926,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J87">
         <v>2.4</v>
@@ -7991,16 +7994,16 @@
         <v>7011577</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D88" s="2">
         <v>45284.20833333334</v>
       </c>
       <c r="E88" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F88" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G88">
         <v>3</v>
@@ -8009,7 +8012,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J88">
         <v>2.2</v>
@@ -8077,16 +8080,16 @@
         <v>7011579</v>
       </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D89" s="2">
         <v>45284.375</v>
       </c>
       <c r="E89" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F89" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G89">
         <v>2</v>
@@ -8095,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J89">
         <v>1.5</v>
@@ -8163,16 +8166,16 @@
         <v>7011578</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D90" s="2">
         <v>45284.47916666666</v>
       </c>
       <c r="E90" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F90" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -8181,7 +8184,7 @@
         <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J90">
         <v>4.3</v>
@@ -8249,16 +8252,16 @@
         <v>7011585</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D91" s="2">
         <v>45312.375</v>
       </c>
       <c r="E91" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F91" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -8267,7 +8270,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J91">
         <v>2.4</v>
@@ -8335,16 +8338,16 @@
         <v>7011584</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D92" s="2">
         <v>45313.33333333334</v>
       </c>
       <c r="E92" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F92" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -8353,7 +8356,7 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J92">
         <v>2.5</v>
@@ -8421,16 +8424,16 @@
         <v>7011583</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D93" s="2">
         <v>45313.4375</v>
       </c>
       <c r="E93" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F93" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G93">
         <v>2</v>
@@ -8439,7 +8442,7 @@
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J93">
         <v>3.4</v>
@@ -8507,16 +8510,16 @@
         <v>7011586</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D94" s="2">
         <v>45314.39583333334</v>
       </c>
       <c r="E94" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F94" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -8525,7 +8528,7 @@
         <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J94">
         <v>2.8</v>
@@ -8593,16 +8596,16 @@
         <v>7011582</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D95" s="2">
         <v>45314.5</v>
       </c>
       <c r="E95" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F95" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G95">
         <v>3</v>
@@ -8611,7 +8614,7 @@
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J95">
         <v>1.222</v>
@@ -8679,16 +8682,16 @@
         <v>7011590</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D96" s="2">
         <v>45317.33333333334</v>
       </c>
       <c r="E96" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F96" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G96">
         <v>3</v>
@@ -8697,7 +8700,7 @@
         <v>1</v>
       </c>
       <c r="I96" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J96">
         <v>1.833</v>
@@ -8765,16 +8768,16 @@
         <v>7011550</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D97" s="2">
         <v>45318.33333333334</v>
       </c>
       <c r="E97" t="s">
+        <v>32</v>
+      </c>
+      <c r="F97" t="s">
         <v>31</v>
-      </c>
-      <c r="F97" t="s">
-        <v>30</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -8783,7 +8786,7 @@
         <v>2</v>
       </c>
       <c r="I97" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J97">
         <v>6.5</v>
@@ -8851,16 +8854,16 @@
         <v>7011589</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D98" s="2">
         <v>45318.4375</v>
       </c>
       <c r="E98" t="s">
+        <v>34</v>
+      </c>
+      <c r="F98" t="s">
         <v>33</v>
-      </c>
-      <c r="F98" t="s">
-        <v>32</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -8869,7 +8872,7 @@
         <v>1</v>
       </c>
       <c r="I98" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J98">
         <v>1.8</v>
@@ -8937,16 +8940,16 @@
         <v>7011587</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D99" s="2">
         <v>45319.33333333334</v>
       </c>
       <c r="E99" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F99" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -8955,7 +8958,7 @@
         <v>1</v>
       </c>
       <c r="I99" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J99">
         <v>2.2</v>
@@ -9023,16 +9026,16 @@
         <v>7011588</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D100" s="2">
         <v>45319.4375</v>
       </c>
       <c r="E100" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F100" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G100">
         <v>3</v>
@@ -9041,7 +9044,7 @@
         <v>1</v>
       </c>
       <c r="I100" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J100">
         <v>1.5</v>
@@ -9109,16 +9112,16 @@
         <v>7011593</v>
       </c>
       <c r="C101" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D101" s="2">
         <v>45325.33333333334</v>
       </c>
       <c r="E101" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F101" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -9127,7 +9130,7 @@
         <v>2</v>
       </c>
       <c r="I101" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J101">
         <v>7</v>
@@ -9195,16 +9198,16 @@
         <v>7011594</v>
       </c>
       <c r="C102" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D102" s="2">
         <v>45325.4375</v>
       </c>
       <c r="E102" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F102" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G102">
         <v>1</v>
@@ -9213,7 +9216,7 @@
         <v>1</v>
       </c>
       <c r="I102" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J102">
         <v>1.727</v>
@@ -9281,16 +9284,16 @@
         <v>7011596</v>
       </c>
       <c r="C103" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D103" s="2">
         <v>45326.33333333334</v>
       </c>
       <c r="E103" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F103" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G103">
         <v>2</v>
@@ -9299,7 +9302,7 @@
         <v>1</v>
       </c>
       <c r="I103" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J103">
         <v>2.4</v>
@@ -9367,16 +9370,16 @@
         <v>7011595</v>
       </c>
       <c r="C104" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D104" s="2">
         <v>45326.4375</v>
       </c>
       <c r="E104" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F104" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G104">
         <v>1</v>
@@ -9385,7 +9388,7 @@
         <v>1</v>
       </c>
       <c r="I104" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J104">
         <v>2.875</v>
@@ -9453,16 +9456,16 @@
         <v>7011592</v>
       </c>
       <c r="C105" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D105" s="2">
         <v>45327.33333333334</v>
       </c>
       <c r="E105" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F105" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G105">
         <v>3</v>
@@ -9471,7 +9474,7 @@
         <v>1</v>
       </c>
       <c r="I105" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J105">
         <v>3.1</v>
@@ -9539,16 +9542,16 @@
         <v>7011601</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D106" s="2">
         <v>45333.5</v>
       </c>
       <c r="E106" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F106" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G106">
         <v>3</v>
@@ -9557,7 +9560,7 @@
         <v>3</v>
       </c>
       <c r="I106" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J106">
         <v>1.444</v>
@@ -9625,16 +9628,16 @@
         <v>7011597</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D107" s="2">
         <v>45334.33333333334</v>
       </c>
       <c r="E107" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F107" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -9643,7 +9646,7 @@
         <v>4</v>
       </c>
       <c r="I107" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J107">
         <v>2.8</v>
@@ -9711,16 +9714,16 @@
         <v>7011600</v>
       </c>
       <c r="C108" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D108" s="2">
         <v>45335.33333333334</v>
       </c>
       <c r="E108" t="s">
+        <v>37</v>
+      </c>
+      <c r="F108" t="s">
         <v>36</v>
-      </c>
-      <c r="F108" t="s">
-        <v>35</v>
       </c>
       <c r="G108">
         <v>2</v>
@@ -9729,7 +9732,7 @@
         <v>1</v>
       </c>
       <c r="I108" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J108">
         <v>1.666</v>
@@ -9797,16 +9800,16 @@
         <v>7011599</v>
       </c>
       <c r="C109" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D109" s="2">
         <v>45335.42708333334</v>
       </c>
       <c r="E109" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F109" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -9815,7 +9818,7 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J109">
         <v>1.8</v>
@@ -9883,16 +9886,16 @@
         <v>7011598</v>
       </c>
       <c r="C110" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D110" s="2">
         <v>45335.52083333334</v>
       </c>
       <c r="E110" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F110" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G110">
         <v>1</v>
@@ -9901,7 +9904,7 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J110">
         <v>2.5</v>
@@ -9969,16 +9972,16 @@
         <v>7011603</v>
       </c>
       <c r="C111" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D111" s="2">
         <v>45339.375</v>
       </c>
       <c r="E111" t="s">
+        <v>33</v>
+      </c>
+      <c r="F111" t="s">
         <v>32</v>
-      </c>
-      <c r="F111" t="s">
-        <v>31</v>
       </c>
       <c r="G111">
         <v>3</v>
@@ -9987,7 +9990,7 @@
         <v>2</v>
       </c>
       <c r="I111" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J111">
         <v>1.666</v>
@@ -10055,17 +10058,17 @@
         <v>7011602</v>
       </c>
       <c r="C112" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D112" s="2">
         <v>45339.47916666666</v>
       </c>
       <c r="E112" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112" t="s">
         <v>29</v>
       </c>
-      <c r="F112" t="s">
-        <v>28</v>
-      </c>
       <c r="G112">
         <v>2</v>
       </c>
@@ -10073,7 +10076,7 @@
         <v>2</v>
       </c>
       <c r="I112" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J112">
         <v>1.8</v>
@@ -10141,17 +10144,17 @@
         <v>7011605</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D113" s="2">
         <v>45340.35416666666</v>
       </c>
       <c r="E113" t="s">
+        <v>38</v>
+      </c>
+      <c r="F113" t="s">
         <v>37</v>
       </c>
-      <c r="F113" t="s">
-        <v>36</v>
-      </c>
       <c r="G113">
         <v>0</v>
       </c>
@@ -10159,7 +10162,7 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J113">
         <v>2.375</v>
@@ -10227,16 +10230,16 @@
         <v>7011606</v>
       </c>
       <c r="C114" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D114" s="2">
         <v>45340.45833333334</v>
       </c>
       <c r="E114" t="s">
+        <v>35</v>
+      </c>
+      <c r="F114" t="s">
         <v>34</v>
-      </c>
-      <c r="F114" t="s">
-        <v>33</v>
       </c>
       <c r="G114">
         <v>1</v>
@@ -10245,7 +10248,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J114">
         <v>2.2</v>
@@ -10313,16 +10316,16 @@
         <v>7011610</v>
       </c>
       <c r="C115" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D115" s="2">
         <v>45345.41666666666</v>
       </c>
       <c r="E115" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F115" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G115">
         <v>2</v>
@@ -10331,7 +10334,7 @@
         <v>1</v>
       </c>
       <c r="I115" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J115">
         <v>2</v>
@@ -10399,16 +10402,16 @@
         <v>7011608</v>
       </c>
       <c r="C116" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D116" s="2">
         <v>45346.33333333334</v>
       </c>
       <c r="E116" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F116" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -10417,7 +10420,7 @@
         <v>1</v>
       </c>
       <c r="I116" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J116">
         <v>3.4</v>
@@ -10485,16 +10488,16 @@
         <v>7011611</v>
       </c>
       <c r="C117" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D117" s="2">
         <v>45346.4375</v>
       </c>
       <c r="E117" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F117" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G117">
         <v>2</v>
@@ -10503,7 +10506,7 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J117">
         <v>2.75</v>
@@ -10571,16 +10574,16 @@
         <v>7011607</v>
       </c>
       <c r="C118" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D118" s="2">
         <v>45347.39583333334</v>
       </c>
       <c r="E118" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F118" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -10589,7 +10592,7 @@
         <v>3</v>
       </c>
       <c r="I118" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J118">
         <v>2.25</v>
@@ -10657,16 +10660,16 @@
         <v>7809824</v>
       </c>
       <c r="C119" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D119" s="2">
         <v>45347.5</v>
       </c>
       <c r="E119" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F119" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G119">
         <v>2</v>
@@ -10675,7 +10678,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J119">
         <v>1.333</v>
@@ -10743,16 +10746,16 @@
         <v>7810273</v>
       </c>
       <c r="C120" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D120" s="2">
         <v>45350.5</v>
       </c>
       <c r="E120" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F120" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -10761,7 +10764,7 @@
         <v>4</v>
       </c>
       <c r="I120" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J120">
         <v>9</v>
@@ -10829,16 +10832,16 @@
         <v>7898044</v>
       </c>
       <c r="C121" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D121" s="2">
         <v>45352.5</v>
       </c>
       <c r="E121" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F121" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G121">
         <v>1</v>
@@ -10847,7 +10850,7 @@
         <v>3</v>
       </c>
       <c r="I121" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J121">
         <v>1.727</v>
@@ -10915,16 +10918,16 @@
         <v>7011616</v>
       </c>
       <c r="C122" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D122" s="2">
         <v>45353.375</v>
       </c>
       <c r="E122" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F122" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G122">
         <v>1</v>
@@ -10933,7 +10936,7 @@
         <v>1</v>
       </c>
       <c r="I122" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J122">
         <v>2.2</v>
@@ -11001,16 +11004,16 @@
         <v>7011612</v>
       </c>
       <c r="C123" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D123" s="2">
         <v>45353.47916666666</v>
       </c>
       <c r="E123" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F123" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G123">
         <v>2</v>
@@ -11019,7 +11022,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J123">
         <v>1.85</v>
@@ -11087,16 +11090,16 @@
         <v>7011613</v>
       </c>
       <c r="C124" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D124" s="2">
         <v>45354.375</v>
       </c>
       <c r="E124" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F124" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G124">
         <v>2</v>
@@ -11105,7 +11108,7 @@
         <v>3</v>
       </c>
       <c r="I124" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J124">
         <v>3.6</v>
@@ -11173,16 +11176,16 @@
         <v>7011615</v>
       </c>
       <c r="C125" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D125" s="2">
         <v>45354.5</v>
       </c>
       <c r="E125" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F125" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -11191,7 +11194,7 @@
         <v>4</v>
       </c>
       <c r="I125" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J125">
         <v>4.75</v>
@@ -11259,16 +11262,16 @@
         <v>7011620</v>
       </c>
       <c r="C126" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D126" s="2">
         <v>45359.5</v>
       </c>
       <c r="E126" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F126" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -11277,7 +11280,7 @@
         <v>1</v>
       </c>
       <c r="I126" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J126">
         <v>2.2</v>
@@ -11345,16 +11348,16 @@
         <v>7011619</v>
       </c>
       <c r="C127" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D127" s="2">
         <v>45360.33333333334</v>
       </c>
       <c r="E127" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F127" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G127">
         <v>3</v>
@@ -11363,7 +11366,7 @@
         <v>3</v>
       </c>
       <c r="I127" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J127">
         <v>3.5</v>
@@ -11431,16 +11434,16 @@
         <v>7011621</v>
       </c>
       <c r="C128" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D128" s="2">
         <v>45360.4375</v>
       </c>
       <c r="E128" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F128" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G128">
         <v>2</v>
@@ -11449,7 +11452,7 @@
         <v>1</v>
       </c>
       <c r="I128" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J128">
         <v>1.4</v>
@@ -11517,16 +11520,16 @@
         <v>7011617</v>
       </c>
       <c r="C129" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D129" s="2">
         <v>45361.35416666666</v>
       </c>
       <c r="E129" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F129" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G129">
         <v>2</v>
@@ -11535,7 +11538,7 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J129">
         <v>2.3</v>
@@ -11603,16 +11606,16 @@
         <v>7011618</v>
       </c>
       <c r="C130" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D130" s="2">
         <v>45361.45833333334</v>
       </c>
       <c r="E130" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F130" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G130">
         <v>3</v>
@@ -11621,7 +11624,7 @@
         <v>1</v>
       </c>
       <c r="I130" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J130">
         <v>1.4</v>
@@ -11689,16 +11692,16 @@
         <v>7011624</v>
       </c>
       <c r="C131" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D131" s="2">
         <v>45366.5</v>
       </c>
       <c r="E131" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F131" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G131">
         <v>3</v>
@@ -11707,7 +11710,7 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J131">
         <v>2.1</v>
@@ -11775,16 +11778,16 @@
         <v>7011625</v>
       </c>
       <c r="C132" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D132" s="2">
         <v>45367.375</v>
       </c>
       <c r="E132" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F132" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G132">
         <v>2</v>
@@ -11793,7 +11796,7 @@
         <v>1</v>
       </c>
       <c r="I132" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J132">
         <v>1.85</v>
@@ -11861,16 +11864,16 @@
         <v>7011622</v>
       </c>
       <c r="C133" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D133" s="2">
         <v>45367.47916666666</v>
       </c>
       <c r="E133" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F133" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -11879,7 +11882,7 @@
         <v>1</v>
       </c>
       <c r="I133" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J133">
         <v>1.85</v>
@@ -11947,16 +11950,16 @@
         <v>7011626</v>
       </c>
       <c r="C134" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D134" s="2">
         <v>45368.375</v>
       </c>
       <c r="E134" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F134" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -11965,7 +11968,7 @@
         <v>3</v>
       </c>
       <c r="I134" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J134">
         <v>4.333</v>
@@ -12033,16 +12036,16 @@
         <v>7011623</v>
       </c>
       <c r="C135" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D135" s="2">
         <v>45368.5</v>
       </c>
       <c r="E135" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F135" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -12051,7 +12054,7 @@
         <v>2</v>
       </c>
       <c r="I135" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J135">
         <v>2.9</v>
@@ -12119,16 +12122,16 @@
         <v>7011628</v>
       </c>
       <c r="C136" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D136" s="2">
         <v>45380.39583333334</v>
       </c>
       <c r="E136" t="s">
+        <v>36</v>
+      </c>
+      <c r="F136" t="s">
         <v>35</v>
-      </c>
-      <c r="F136" t="s">
-        <v>34</v>
       </c>
       <c r="G136">
         <v>0</v>
@@ -12137,7 +12140,7 @@
         <v>1</v>
       </c>
       <c r="I136" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J136">
         <v>3.5</v>
@@ -12205,16 +12208,16 @@
         <v>7011631</v>
       </c>
       <c r="C137" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D137" s="2">
         <v>45380.5</v>
       </c>
       <c r="E137" t="s">
+        <v>32</v>
+      </c>
+      <c r="F137" t="s">
         <v>31</v>
-      </c>
-      <c r="F137" t="s">
-        <v>30</v>
       </c>
       <c r="G137">
         <v>1</v>
@@ -12223,7 +12226,7 @@
         <v>6</v>
       </c>
       <c r="I137" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J137">
         <v>6</v>
@@ -12291,16 +12294,16 @@
         <v>7011630</v>
       </c>
       <c r="C138" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D138" s="2">
         <v>45381.39583333334</v>
       </c>
       <c r="E138" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F138" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -12309,7 +12312,7 @@
         <v>1</v>
       </c>
       <c r="I138" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J138">
         <v>2.3</v>
@@ -12377,16 +12380,16 @@
         <v>7011629</v>
       </c>
       <c r="C139" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D139" s="2">
         <v>45381.5</v>
       </c>
       <c r="E139" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F139" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -12395,7 +12398,7 @@
         <v>1</v>
       </c>
       <c r="I139" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J139">
         <v>2.1</v>
@@ -12463,16 +12466,16 @@
         <v>7011627</v>
       </c>
       <c r="C140" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D140" s="2">
         <v>45382.45833333334</v>
       </c>
       <c r="E140" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F140" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -12481,7 +12484,7 @@
         <v>0</v>
       </c>
       <c r="I140" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J140">
         <v>1.95</v>
@@ -12549,16 +12552,16 @@
         <v>7011632</v>
       </c>
       <c r="C141" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D141" s="2">
         <v>45387.54166666666</v>
       </c>
       <c r="E141" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F141" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -12567,7 +12570,7 @@
         <v>2</v>
       </c>
       <c r="I141" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J141">
         <v>2.1</v>
@@ -12635,16 +12638,16 @@
         <v>7011634</v>
       </c>
       <c r="C142" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D142" s="2">
         <v>45388.375</v>
       </c>
       <c r="E142" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F142" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G142">
         <v>2</v>
@@ -12653,7 +12656,7 @@
         <v>0</v>
       </c>
       <c r="I142" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J142">
         <v>2.55</v>
@@ -12721,16 +12724,16 @@
         <v>7011633</v>
       </c>
       <c r="C143" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D143" s="2">
         <v>45388.54166666666</v>
       </c>
       <c r="E143" t="s">
+        <v>31</v>
+      </c>
+      <c r="F143" t="s">
         <v>30</v>
-      </c>
-      <c r="F143" t="s">
-        <v>29</v>
       </c>
       <c r="G143">
         <v>4</v>
@@ -12739,7 +12742,7 @@
         <v>2</v>
       </c>
       <c r="I143" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J143">
         <v>1.222</v>
@@ -12807,16 +12810,16 @@
         <v>7011635</v>
       </c>
       <c r="C144" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D144" s="2">
         <v>45389.39583333334</v>
       </c>
       <c r="E144" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F144" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G144">
         <v>4</v>
@@ -12825,7 +12828,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J144">
         <v>1.4</v>
@@ -12893,16 +12896,16 @@
         <v>7011636</v>
       </c>
       <c r="C145" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D145" s="2">
         <v>45389.54166666666</v>
       </c>
       <c r="E145" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F145" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G145">
         <v>1</v>
@@ -12911,7 +12914,7 @@
         <v>1</v>
       </c>
       <c r="I145" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J145">
         <v>1.727</v>
@@ -12979,16 +12982,16 @@
         <v>7011638</v>
       </c>
       <c r="C146" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D146" s="2">
         <v>45394.5</v>
       </c>
       <c r="E146" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F146" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G146">
         <v>0</v>
@@ -12997,7 +13000,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J146">
         <v>2.9</v>
@@ -13065,16 +13068,16 @@
         <v>7011639</v>
       </c>
       <c r="C147" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D147" s="2">
         <v>45395.39583333334</v>
       </c>
       <c r="E147" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F147" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G147">
         <v>1</v>
@@ -13083,7 +13086,7 @@
         <v>2</v>
       </c>
       <c r="I147" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J147">
         <v>3</v>
@@ -13151,16 +13154,16 @@
         <v>7011637</v>
       </c>
       <c r="C148" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D148" s="2">
         <v>45395.5</v>
       </c>
       <c r="E148" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F148" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G148">
         <v>3</v>
@@ -13169,7 +13172,7 @@
         <v>0</v>
       </c>
       <c r="I148" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J148">
         <v>1.833</v>
@@ -13237,16 +13240,16 @@
         <v>7011640</v>
       </c>
       <c r="C149" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D149" s="2">
         <v>45396.39583333334</v>
       </c>
       <c r="E149" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F149" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G149">
         <v>3</v>
@@ -13255,7 +13258,7 @@
         <v>3</v>
       </c>
       <c r="I149" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J149">
         <v>1.727</v>
@@ -13323,16 +13326,16 @@
         <v>7012356</v>
       </c>
       <c r="C150" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D150" s="2">
         <v>45396.5</v>
       </c>
       <c r="E150" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F150" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G150">
         <v>3</v>
@@ -13341,7 +13344,7 @@
         <v>2</v>
       </c>
       <c r="I150" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J150">
         <v>2.625</v>
@@ -13409,16 +13412,16 @@
         <v>7020807</v>
       </c>
       <c r="C151" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D151" s="2">
         <v>45401.39583333334</v>
       </c>
       <c r="E151" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F151" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G151">
         <v>1</v>
@@ -13427,7 +13430,7 @@
         <v>4</v>
       </c>
       <c r="I151" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J151">
         <v>2.25</v>
@@ -13495,16 +13498,16 @@
         <v>7029131</v>
       </c>
       <c r="C152" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D152" s="2">
         <v>45402.39583333334</v>
       </c>
       <c r="E152" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F152" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G152">
         <v>2</v>
@@ -13513,7 +13516,7 @@
         <v>2</v>
       </c>
       <c r="I152" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J152">
         <v>1.166</v>
@@ -13581,16 +13584,16 @@
         <v>7025505</v>
       </c>
       <c r="C153" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D153" s="2">
         <v>45402.5</v>
       </c>
       <c r="E153" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F153" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G153">
         <v>3</v>
@@ -13599,7 +13602,7 @@
         <v>1</v>
       </c>
       <c r="I153" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J153">
         <v>2.1</v>
@@ -13667,16 +13670,16 @@
         <v>7027687</v>
       </c>
       <c r="C154" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D154" s="2">
         <v>45403.39583333334</v>
       </c>
       <c r="E154" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F154" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G154">
         <v>1</v>
@@ -13685,7 +13688,7 @@
         <v>2</v>
       </c>
       <c r="I154" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J154">
         <v>2.75</v>
@@ -13753,16 +13756,16 @@
         <v>7020806</v>
       </c>
       <c r="C155" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D155" s="2">
         <v>45403.5</v>
       </c>
       <c r="E155" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F155" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G155">
         <v>0</v>
@@ -13771,7 +13774,7 @@
         <v>2</v>
       </c>
       <c r="I155" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J155">
         <v>2.5</v>
@@ -13829,6 +13832,71 @@
       </c>
       <c r="AB155">
         <v>0.875</v>
+      </c>
+    </row>
+    <row r="156" spans="1:28">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>27</v>
+      </c>
+      <c r="C156" t="s">
+        <v>28</v>
+      </c>
+      <c r="D156" s="2">
+        <v>45409.45833333334</v>
+      </c>
+      <c r="E156" t="s">
+        <v>33</v>
+      </c>
+      <c r="F156" t="s">
+        <v>30</v>
+      </c>
+      <c r="J156">
+        <v>1.85</v>
+      </c>
+      <c r="K156">
+        <v>3.4</v>
+      </c>
+      <c r="L156">
+        <v>3.6</v>
+      </c>
+      <c r="M156">
+        <v>1.85</v>
+      </c>
+      <c r="N156">
+        <v>3.4</v>
+      </c>
+      <c r="O156">
+        <v>3.6</v>
+      </c>
+      <c r="P156">
+        <v>-0.5</v>
+      </c>
+      <c r="Q156">
+        <v>1.9</v>
+      </c>
+      <c r="R156">
+        <v>1.9</v>
+      </c>
+      <c r="S156">
+        <v>2.5</v>
+      </c>
+      <c r="T156">
+        <v>1.85</v>
+      </c>
+      <c r="U156">
+        <v>1.95</v>
+      </c>
+      <c r="V156">
+        <v>0</v>
+      </c>
+      <c r="W156">
+        <v>0</v>
+      </c>
+      <c r="X156">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 28-04-2024 às 15:37
</commit_message>
<xml_diff>
--- a/Azerbaijan Premier League/Azerbaijan Premier League.xlsx
+++ b/Azerbaijan Premier League/Azerbaijan Premier League.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -97,7 +97,13 @@
     <t>PL_AhUnder</t>
   </si>
   <si>
-    <t>7071263</t>
+    <t>7065195</t>
+  </si>
+  <si>
+    <t>7062589</t>
+  </si>
+  <si>
+    <t>7060565</t>
   </si>
   <si>
     <t>Azerbaijan Premier League</t>
@@ -501,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB156"/>
+  <dimension ref="A1:AB158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -598,16 +604,16 @@
         <v>6943460</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2">
         <v>45142.54166666666</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -616,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J2">
         <v>2.1</v>
@@ -684,16 +690,16 @@
         <v>6943462</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2">
         <v>45143.47916666666</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -702,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -770,16 +776,16 @@
         <v>6942350</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2">
         <v>45143.58333333334</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -788,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J4">
         <v>1.181</v>
@@ -856,16 +862,16 @@
         <v>6943461</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2">
         <v>45144.41666666666</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -874,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -942,16 +948,16 @@
         <v>6940298</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2">
         <v>45144.54166666666</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -960,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J6">
         <v>1.571</v>
@@ -1028,16 +1034,16 @@
         <v>6943463</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2">
         <v>45150.47916666666</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1046,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -1114,16 +1120,16 @@
         <v>6943465</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2">
         <v>45150.58333333334</v>
       </c>
       <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1132,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J8">
         <v>1.571</v>
@@ -1200,16 +1206,16 @@
         <v>6942351</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2">
         <v>45151.47916666666</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -1218,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J9">
         <v>1.533</v>
@@ -1286,16 +1292,16 @@
         <v>6943464</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2">
         <v>45152.54166666666</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1304,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>1.5</v>
@@ -1372,16 +1378,16 @@
         <v>6943466</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2">
         <v>45156.41666666666</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1390,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J11">
         <v>2.3</v>
@@ -1458,16 +1464,16 @@
         <v>6943468</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2">
         <v>45157.45833333334</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1476,7 +1482,7 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J12">
         <v>2.1</v>
@@ -1544,16 +1550,16 @@
         <v>6943467</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2">
         <v>45157.54166666666</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1562,7 +1568,7 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J13">
         <v>3.5</v>
@@ -1630,16 +1636,16 @@
         <v>6944562</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2">
         <v>45158.45833333334</v>
       </c>
       <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
         <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1648,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J14">
         <v>1.166</v>
@@ -1716,16 +1722,16 @@
         <v>6940300</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2">
         <v>45158.54166666666</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1734,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J15">
         <v>1.5</v>
@@ -1802,16 +1808,16 @@
         <v>6943469</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2">
         <v>45163.54166666666</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1820,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J16">
         <v>2.4</v>
@@ -1888,16 +1894,16 @@
         <v>6943471</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2">
         <v>45164.41666666666</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1906,7 +1912,7 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J17">
         <v>2.4</v>
@@ -1974,16 +1980,16 @@
         <v>6940301</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2">
         <v>45164.52083333334</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1992,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J18">
         <v>3.1</v>
@@ -2060,16 +2066,16 @@
         <v>6943470</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2">
         <v>45165.47916666666</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -2078,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J19">
         <v>1.833</v>
@@ -2146,16 +2152,16 @@
         <v>6942352</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2">
         <v>45165.57291666666</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2164,7 +2170,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J20">
         <v>1.166</v>
@@ -2232,16 +2238,16 @@
         <v>6940302</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2">
         <v>45170.5</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2250,7 +2256,7 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J21">
         <v>1.444</v>
@@ -2318,16 +2324,16 @@
         <v>6943473</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D22" s="2">
         <v>45171.45833333334</v>
       </c>
       <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
         <v>36</v>
-      </c>
-      <c r="F22" t="s">
-        <v>34</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2336,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J22">
         <v>4.333</v>
@@ -2404,16 +2410,16 @@
         <v>6943474</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D23" s="2">
         <v>45171.5625</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2422,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J23">
         <v>4.75</v>
@@ -2490,16 +2496,16 @@
         <v>6943472</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2">
         <v>45172.41666666666</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2508,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J24">
         <v>2.375</v>
@@ -2576,16 +2582,16 @@
         <v>6942353</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2">
         <v>45172.52083333334</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G25">
         <v>2</v>
@@ -2594,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J25">
         <v>9</v>
@@ -2662,16 +2668,16 @@
         <v>6976494</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D26" s="2">
         <v>45184.41666666666</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2680,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J26">
         <v>1.6</v>
@@ -2748,16 +2754,16 @@
         <v>6976497</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D27" s="2">
         <v>45185.375</v>
       </c>
       <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
         <v>32</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2766,7 +2772,7 @@
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J27">
         <v>2.5</v>
@@ -2834,16 +2840,16 @@
         <v>6976493</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D28" s="2">
         <v>45185.45833333334</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2852,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J28">
         <v>5</v>
@@ -2920,16 +2926,16 @@
         <v>6976495</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2">
         <v>45186.39583333334</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -2938,7 +2944,7 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J29">
         <v>2.5</v>
@@ -3006,16 +3012,16 @@
         <v>6976496</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2">
         <v>45186.52083333334</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -3024,7 +3030,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J30">
         <v>1.533</v>
@@ -3092,16 +3098,16 @@
         <v>6976500</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D31" s="2">
         <v>45192.45833333334</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3110,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J31">
         <v>2.55</v>
@@ -3178,16 +3184,16 @@
         <v>6977259</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2">
         <v>45193.41666666666</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G32">
         <v>2</v>
@@ -3196,7 +3202,7 @@
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J32">
         <v>1.533</v>
@@ -3264,16 +3270,16 @@
         <v>6976498</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D33" s="2">
         <v>45193.52083333334</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -3282,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J33">
         <v>2.3</v>
@@ -3350,16 +3356,16 @@
         <v>6976499</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D34" s="2">
         <v>45194.5</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -3368,7 +3374,7 @@
         <v>2</v>
       </c>
       <c r="I34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J34">
         <v>6.5</v>
@@ -3436,16 +3442,16 @@
         <v>6976504</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D35" s="2">
         <v>45198.54166666666</v>
       </c>
       <c r="E35" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G35">
         <v>5</v>
@@ -3454,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J35">
         <v>1.285</v>
@@ -3522,16 +3528,16 @@
         <v>6976503</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D36" s="2">
         <v>45199.375</v>
       </c>
       <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" t="s">
         <v>37</v>
-      </c>
-      <c r="F36" t="s">
-        <v>35</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -3540,7 +3546,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J36">
         <v>2.5</v>
@@ -3608,16 +3614,16 @@
         <v>6976506</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D37" s="2">
         <v>45199.45833333334</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G37">
         <v>2</v>
@@ -3626,7 +3632,7 @@
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J37">
         <v>2.8</v>
@@ -3694,16 +3700,16 @@
         <v>6976505</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D38" s="2">
         <v>45200.375</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3712,7 +3718,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J38">
         <v>2.375</v>
@@ -3780,16 +3786,16 @@
         <v>6976502</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D39" s="2">
         <v>45200.47916666666</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F39" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -3798,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J39">
         <v>2.5</v>
@@ -3866,16 +3872,16 @@
         <v>7011536</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D40" s="2">
         <v>45205.45833333334</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G40">
         <v>2</v>
@@ -3884,7 +3890,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J40">
         <v>1.5</v>
@@ -3952,16 +3958,16 @@
         <v>7011533</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D41" s="2">
         <v>45206.375</v>
       </c>
       <c r="E41" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -3970,7 +3976,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J41">
         <v>2.25</v>
@@ -4038,16 +4044,16 @@
         <v>7011532</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D42" s="2">
         <v>45206.45833333334</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -4056,7 +4062,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J42">
         <v>1.8</v>
@@ -4124,16 +4130,16 @@
         <v>7011534</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D43" s="2">
         <v>45207.39583333334</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -4142,7 +4148,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J43">
         <v>2.25</v>
@@ -4210,16 +4216,16 @@
         <v>7011535</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D44" s="2">
         <v>45207.52083333334</v>
       </c>
       <c r="E44" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F44" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -4228,7 +4234,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J44">
         <v>4.8</v>
@@ -4296,16 +4302,16 @@
         <v>7011541</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D45" s="2">
         <v>45219.47916666666</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F45" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G45">
         <v>2</v>
@@ -4314,7 +4320,7 @@
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J45">
         <v>7</v>
@@ -4382,16 +4388,16 @@
         <v>7011539</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D46" s="2">
         <v>45219.5625</v>
       </c>
       <c r="E46" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F46" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -4400,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J46">
         <v>3</v>
@@ -4468,16 +4474,16 @@
         <v>7011540</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D47" s="2">
         <v>45220.33333333334</v>
       </c>
       <c r="E47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -4486,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J47">
         <v>5.5</v>
@@ -4554,16 +4560,16 @@
         <v>7011538</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D48" s="2">
         <v>45220.45833333334</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F48" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G48">
         <v>3</v>
@@ -4572,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J48">
         <v>1.75</v>
@@ -4640,16 +4646,16 @@
         <v>7011537</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D49" s="2">
         <v>45221.39583333334</v>
       </c>
       <c r="E49" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -4658,7 +4664,7 @@
         <v>4</v>
       </c>
       <c r="I49" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J49">
         <v>2</v>
@@ -4726,16 +4732,16 @@
         <v>7267423</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D50" s="2">
         <v>45224.47916666666</v>
       </c>
       <c r="E50" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F50" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -4744,7 +4750,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J50">
         <v>5</v>
@@ -4812,16 +4818,16 @@
         <v>7011544</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D51" s="2">
         <v>45227.375</v>
       </c>
       <c r="E51" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G51">
         <v>2</v>
@@ -4830,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J51">
         <v>2</v>
@@ -4898,16 +4904,16 @@
         <v>7011543</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D52" s="2">
         <v>45227.5</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F52" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G52">
         <v>4</v>
@@ -4916,7 +4922,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J52">
         <v>2.25</v>
@@ -4984,17 +4990,17 @@
         <v>7011546</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D53" s="2">
         <v>45228.375</v>
       </c>
       <c r="E53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" t="s">
         <v>38</v>
       </c>
-      <c r="F53" t="s">
-        <v>36</v>
-      </c>
       <c r="G53">
         <v>0</v>
       </c>
@@ -5002,7 +5008,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J53">
         <v>2.2</v>
@@ -5070,16 +5076,16 @@
         <v>7011545</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D54" s="2">
         <v>45228.47916666666</v>
       </c>
       <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" t="s">
         <v>35</v>
-      </c>
-      <c r="F54" t="s">
-        <v>33</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -5088,7 +5094,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J54">
         <v>2.5</v>
@@ -5156,16 +5162,16 @@
         <v>7011542</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D55" s="2">
         <v>45229.5</v>
       </c>
       <c r="E55" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F55" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G55">
         <v>2</v>
@@ -5174,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J55">
         <v>5.75</v>
@@ -5242,16 +5248,16 @@
         <v>7011549</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D56" s="2">
         <v>45233.5</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -5260,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J56">
         <v>2.25</v>
@@ -5328,16 +5334,16 @@
         <v>7011591</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D57" s="2">
         <v>45234.375</v>
       </c>
       <c r="E57" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F57" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G57">
         <v>7</v>
@@ -5346,7 +5352,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J57">
         <v>1.125</v>
@@ -5414,16 +5420,16 @@
         <v>7011547</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D58" s="2">
         <v>45234.45833333334</v>
       </c>
       <c r="E58" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F58" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G58">
         <v>2</v>
@@ -5432,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J58">
         <v>2.75</v>
@@ -5500,16 +5506,16 @@
         <v>7011551</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D59" s="2">
         <v>45235.375</v>
       </c>
       <c r="E59" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F59" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -5518,7 +5524,7 @@
         <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J59">
         <v>3.6</v>
@@ -5586,16 +5592,16 @@
         <v>7011548</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D60" s="2">
         <v>45235.47916666666</v>
       </c>
       <c r="E60" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F60" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -5604,7 +5610,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J60">
         <v>2.25</v>
@@ -5672,16 +5678,16 @@
         <v>7011552</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D61" s="2">
         <v>45240.5</v>
       </c>
       <c r="E61" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F61" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -5690,7 +5696,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J61">
         <v>1.4</v>
@@ -5758,16 +5764,16 @@
         <v>7011556</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D62" s="2">
         <v>45241.39583333334</v>
       </c>
       <c r="E62" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F62" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -5776,7 +5782,7 @@
         <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J62">
         <v>1.5</v>
@@ -5844,16 +5850,16 @@
         <v>7011554</v>
       </c>
       <c r="C63" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D63" s="2">
         <v>45241.5</v>
       </c>
       <c r="E63" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F63" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -5862,7 +5868,7 @@
         <v>3</v>
       </c>
       <c r="I63" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J63">
         <v>3.1</v>
@@ -5930,16 +5936,16 @@
         <v>7011555</v>
       </c>
       <c r="C64" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D64" s="2">
         <v>45242.39583333334</v>
       </c>
       <c r="E64" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F64" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -5948,7 +5954,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J64">
         <v>1.95</v>
@@ -6016,16 +6022,16 @@
         <v>7011553</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D65" s="2">
         <v>45242.5</v>
       </c>
       <c r="E65" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G65">
         <v>3</v>
@@ -6034,7 +6040,7 @@
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J65">
         <v>1.222</v>
@@ -6102,16 +6108,16 @@
         <v>7011560</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D66" s="2">
         <v>45254.54166666666</v>
       </c>
       <c r="E66" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" t="s">
         <v>33</v>
-      </c>
-      <c r="F66" t="s">
-        <v>31</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -6120,7 +6126,7 @@
         <v>2</v>
       </c>
       <c r="I66" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J66">
         <v>4</v>
@@ -6188,16 +6194,16 @@
         <v>7011561</v>
       </c>
       <c r="C67" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D67" s="2">
         <v>45255.29166666666</v>
       </c>
       <c r="E67" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F67" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -6206,7 +6212,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J67">
         <v>1.65</v>
@@ -6274,16 +6280,16 @@
         <v>7011559</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D68" s="2">
         <v>45255.375</v>
       </c>
       <c r="E68" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F68" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G68">
         <v>4</v>
@@ -6292,7 +6298,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J68">
         <v>2.2</v>
@@ -6360,16 +6366,16 @@
         <v>7011557</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D69" s="2">
         <v>45256.35416666666</v>
       </c>
       <c r="E69" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F69" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -6378,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J69">
         <v>1.6</v>
@@ -6446,16 +6452,16 @@
         <v>7011558</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D70" s="2">
         <v>45256.45833333334</v>
       </c>
       <c r="E70" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F70" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -6464,7 +6470,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J70">
         <v>3.1</v>
@@ -6532,16 +6538,16 @@
         <v>7011562</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D71" s="2">
         <v>45262.375</v>
       </c>
       <c r="E71" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F71" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -6550,7 +6556,7 @@
         <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J71">
         <v>2.2</v>
@@ -6618,16 +6624,16 @@
         <v>7011565</v>
       </c>
       <c r="C72" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D72" s="2">
         <v>45262.47916666666</v>
       </c>
       <c r="E72" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F72" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G72">
         <v>2</v>
@@ -6636,7 +6642,7 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J72">
         <v>2.375</v>
@@ -6704,16 +6710,16 @@
         <v>7011563</v>
       </c>
       <c r="C73" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D73" s="2">
         <v>45263.33333333334</v>
       </c>
       <c r="E73" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F73" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -6722,7 +6728,7 @@
         <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J73">
         <v>3.6</v>
@@ -6790,16 +6796,16 @@
         <v>7011566</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D74" s="2">
         <v>45263.41666666666</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -6808,7 +6814,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J74">
         <v>2</v>
@@ -6876,16 +6882,16 @@
         <v>7011564</v>
       </c>
       <c r="C75" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D75" s="2">
         <v>45264.52083333334</v>
       </c>
       <c r="E75" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F75" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G75">
         <v>3</v>
@@ -6894,7 +6900,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J75">
         <v>1.181</v>
@@ -6962,16 +6968,16 @@
         <v>7011569</v>
       </c>
       <c r="C76" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D76" s="2">
         <v>45268.52083333334</v>
       </c>
       <c r="E76" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F76" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -6980,7 +6986,7 @@
         <v>6</v>
       </c>
       <c r="I76" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J76">
         <v>4.333</v>
@@ -7048,16 +7054,16 @@
         <v>7011570</v>
       </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D77" s="2">
         <v>45269.33333333334</v>
       </c>
       <c r="E77" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F77" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -7066,7 +7072,7 @@
         <v>3</v>
       </c>
       <c r="I77" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J77">
         <v>1.727</v>
@@ -7134,16 +7140,16 @@
         <v>7011567</v>
       </c>
       <c r="C78" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D78" s="2">
         <v>45269.41666666666</v>
       </c>
       <c r="E78" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F78" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -7152,7 +7158,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J78">
         <v>1.666</v>
@@ -7220,16 +7226,16 @@
         <v>7011571</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D79" s="2">
         <v>45270.33333333334</v>
       </c>
       <c r="E79" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F79" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G79">
         <v>4</v>
@@ -7238,7 +7244,7 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J79">
         <v>1.615</v>
@@ -7306,16 +7312,16 @@
         <v>7011568</v>
       </c>
       <c r="C80" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D80" s="2">
         <v>45270.45833333334</v>
       </c>
       <c r="E80" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F80" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G80">
         <v>3</v>
@@ -7324,7 +7330,7 @@
         <v>2</v>
       </c>
       <c r="I80" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J80">
         <v>2</v>
@@ -7392,16 +7398,16 @@
         <v>7011574</v>
       </c>
       <c r="C81" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D81" s="2">
         <v>45274.35416666666</v>
       </c>
       <c r="E81" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F81" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -7410,7 +7416,7 @@
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J81">
         <v>2.625</v>
@@ -7478,16 +7484,16 @@
         <v>7011573</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D82" s="2">
         <v>45275.25</v>
       </c>
       <c r="E82" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F82" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G82">
         <v>3</v>
@@ -7496,7 +7502,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J82">
         <v>2.1</v>
@@ -7564,16 +7570,16 @@
         <v>7011572</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D83" s="2">
         <v>45275.33333333334</v>
       </c>
       <c r="E83" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F83" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G83">
         <v>2</v>
@@ -7582,7 +7588,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J83">
         <v>2.3</v>
@@ -7650,16 +7656,16 @@
         <v>7011576</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D84" s="2">
         <v>45276.45833333334</v>
       </c>
       <c r="E84" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F84" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -7668,7 +7674,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J84">
         <v>3</v>
@@ -7736,16 +7742,16 @@
         <v>7011575</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D85" s="2">
         <v>45278.54166666666</v>
       </c>
       <c r="E85" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F85" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G85">
         <v>2</v>
@@ -7754,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J85">
         <v>1.363</v>
@@ -7822,16 +7828,16 @@
         <v>7011581</v>
       </c>
       <c r="C86" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D86" s="2">
         <v>45282.375</v>
       </c>
       <c r="E86" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F86" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -7840,7 +7846,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J86">
         <v>4</v>
@@ -7908,16 +7914,16 @@
         <v>7011580</v>
       </c>
       <c r="C87" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D87" s="2">
         <v>45283.47916666666</v>
       </c>
       <c r="E87" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F87" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -7926,7 +7932,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J87">
         <v>2.4</v>
@@ -7994,16 +8000,16 @@
         <v>7011577</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D88" s="2">
         <v>45284.20833333334</v>
       </c>
       <c r="E88" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F88" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G88">
         <v>3</v>
@@ -8012,7 +8018,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J88">
         <v>2.2</v>
@@ -8080,16 +8086,16 @@
         <v>7011579</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D89" s="2">
         <v>45284.375</v>
       </c>
       <c r="E89" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F89" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G89">
         <v>2</v>
@@ -8098,7 +8104,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J89">
         <v>1.5</v>
@@ -8166,16 +8172,16 @@
         <v>7011578</v>
       </c>
       <c r="C90" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D90" s="2">
         <v>45284.47916666666</v>
       </c>
       <c r="E90" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F90" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -8184,7 +8190,7 @@
         <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J90">
         <v>4.3</v>
@@ -8252,16 +8258,16 @@
         <v>7011585</v>
       </c>
       <c r="C91" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D91" s="2">
         <v>45312.375</v>
       </c>
       <c r="E91" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F91" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -8270,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J91">
         <v>2.4</v>
@@ -8338,16 +8344,16 @@
         <v>7011584</v>
       </c>
       <c r="C92" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D92" s="2">
         <v>45313.33333333334</v>
       </c>
       <c r="E92" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F92" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -8356,7 +8362,7 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J92">
         <v>2.5</v>
@@ -8424,16 +8430,16 @@
         <v>7011583</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D93" s="2">
         <v>45313.4375</v>
       </c>
       <c r="E93" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F93" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G93">
         <v>2</v>
@@ -8442,7 +8448,7 @@
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J93">
         <v>3.4</v>
@@ -8510,16 +8516,16 @@
         <v>7011586</v>
       </c>
       <c r="C94" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D94" s="2">
         <v>45314.39583333334</v>
       </c>
       <c r="E94" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F94" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -8528,7 +8534,7 @@
         <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J94">
         <v>2.8</v>
@@ -8596,16 +8602,16 @@
         <v>7011582</v>
       </c>
       <c r="C95" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D95" s="2">
         <v>45314.5</v>
       </c>
       <c r="E95" t="s">
+        <v>33</v>
+      </c>
+      <c r="F95" t="s">
         <v>31</v>
-      </c>
-      <c r="F95" t="s">
-        <v>29</v>
       </c>
       <c r="G95">
         <v>3</v>
@@ -8614,7 +8620,7 @@
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J95">
         <v>1.222</v>
@@ -8682,16 +8688,16 @@
         <v>7011590</v>
       </c>
       <c r="C96" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D96" s="2">
         <v>45317.33333333334</v>
       </c>
       <c r="E96" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F96" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G96">
         <v>3</v>
@@ -8700,7 +8706,7 @@
         <v>1</v>
       </c>
       <c r="I96" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J96">
         <v>1.833</v>
@@ -8768,16 +8774,16 @@
         <v>7011550</v>
       </c>
       <c r="C97" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D97" s="2">
         <v>45318.33333333334</v>
       </c>
       <c r="E97" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F97" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -8786,7 +8792,7 @@
         <v>2</v>
       </c>
       <c r="I97" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J97">
         <v>6.5</v>
@@ -8854,16 +8860,16 @@
         <v>7011589</v>
       </c>
       <c r="C98" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D98" s="2">
         <v>45318.4375</v>
       </c>
       <c r="E98" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F98" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -8872,7 +8878,7 @@
         <v>1</v>
       </c>
       <c r="I98" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J98">
         <v>1.8</v>
@@ -8940,16 +8946,16 @@
         <v>7011587</v>
       </c>
       <c r="C99" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D99" s="2">
         <v>45319.33333333334</v>
       </c>
       <c r="E99" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F99" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -8958,7 +8964,7 @@
         <v>1</v>
       </c>
       <c r="I99" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J99">
         <v>2.2</v>
@@ -9026,16 +9032,16 @@
         <v>7011588</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D100" s="2">
         <v>45319.4375</v>
       </c>
       <c r="E100" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F100" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G100">
         <v>3</v>
@@ -9044,7 +9050,7 @@
         <v>1</v>
       </c>
       <c r="I100" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J100">
         <v>1.5</v>
@@ -9112,16 +9118,16 @@
         <v>7011593</v>
       </c>
       <c r="C101" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D101" s="2">
         <v>45325.33333333334</v>
       </c>
       <c r="E101" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F101" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -9130,7 +9136,7 @@
         <v>2</v>
       </c>
       <c r="I101" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J101">
         <v>7</v>
@@ -9198,16 +9204,16 @@
         <v>7011594</v>
       </c>
       <c r="C102" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D102" s="2">
         <v>45325.4375</v>
       </c>
       <c r="E102" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F102" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G102">
         <v>1</v>
@@ -9216,7 +9222,7 @@
         <v>1</v>
       </c>
       <c r="I102" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J102">
         <v>1.727</v>
@@ -9284,16 +9290,16 @@
         <v>7011596</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D103" s="2">
         <v>45326.33333333334</v>
       </c>
       <c r="E103" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F103" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G103">
         <v>2</v>
@@ -9302,7 +9308,7 @@
         <v>1</v>
       </c>
       <c r="I103" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J103">
         <v>2.4</v>
@@ -9370,16 +9376,16 @@
         <v>7011595</v>
       </c>
       <c r="C104" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D104" s="2">
         <v>45326.4375</v>
       </c>
       <c r="E104" t="s">
+        <v>38</v>
+      </c>
+      <c r="F104" t="s">
         <v>36</v>
-      </c>
-      <c r="F104" t="s">
-        <v>34</v>
       </c>
       <c r="G104">
         <v>1</v>
@@ -9388,7 +9394,7 @@
         <v>1</v>
       </c>
       <c r="I104" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J104">
         <v>2.875</v>
@@ -9456,16 +9462,16 @@
         <v>7011592</v>
       </c>
       <c r="C105" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D105" s="2">
         <v>45327.33333333334</v>
       </c>
       <c r="E105" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F105" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G105">
         <v>3</v>
@@ -9474,7 +9480,7 @@
         <v>1</v>
       </c>
       <c r="I105" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J105">
         <v>3.1</v>
@@ -9542,16 +9548,16 @@
         <v>7011601</v>
       </c>
       <c r="C106" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D106" s="2">
         <v>45333.5</v>
       </c>
       <c r="E106" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F106" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G106">
         <v>3</v>
@@ -9560,7 +9566,7 @@
         <v>3</v>
       </c>
       <c r="I106" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J106">
         <v>1.444</v>
@@ -9628,16 +9634,16 @@
         <v>7011597</v>
       </c>
       <c r="C107" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D107" s="2">
         <v>45334.33333333334</v>
       </c>
       <c r="E107" t="s">
+        <v>34</v>
+      </c>
+      <c r="F107" t="s">
         <v>32</v>
-      </c>
-      <c r="F107" t="s">
-        <v>30</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -9646,7 +9652,7 @@
         <v>4</v>
       </c>
       <c r="I107" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J107">
         <v>2.8</v>
@@ -9714,16 +9720,16 @@
         <v>7011600</v>
       </c>
       <c r="C108" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D108" s="2">
         <v>45335.33333333334</v>
       </c>
       <c r="E108" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F108" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G108">
         <v>2</v>
@@ -9732,7 +9738,7 @@
         <v>1</v>
       </c>
       <c r="I108" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J108">
         <v>1.666</v>
@@ -9800,16 +9806,16 @@
         <v>7011599</v>
       </c>
       <c r="C109" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D109" s="2">
         <v>45335.42708333334</v>
       </c>
       <c r="E109" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F109" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -9818,7 +9824,7 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J109">
         <v>1.8</v>
@@ -9886,16 +9892,16 @@
         <v>7011598</v>
       </c>
       <c r="C110" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D110" s="2">
         <v>45335.52083333334</v>
       </c>
       <c r="E110" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F110" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G110">
         <v>1</v>
@@ -9904,7 +9910,7 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J110">
         <v>2.5</v>
@@ -9972,16 +9978,16 @@
         <v>7011603</v>
       </c>
       <c r="C111" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D111" s="2">
         <v>45339.375</v>
       </c>
       <c r="E111" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F111" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G111">
         <v>3</v>
@@ -9990,7 +9996,7 @@
         <v>2</v>
       </c>
       <c r="I111" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J111">
         <v>1.666</v>
@@ -10058,16 +10064,16 @@
         <v>7011602</v>
       </c>
       <c r="C112" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D112" s="2">
         <v>45339.47916666666</v>
       </c>
       <c r="E112" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F112" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G112">
         <v>2</v>
@@ -10076,7 +10082,7 @@
         <v>2</v>
       </c>
       <c r="I112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J112">
         <v>1.8</v>
@@ -10144,16 +10150,16 @@
         <v>7011605</v>
       </c>
       <c r="C113" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D113" s="2">
         <v>45340.35416666666</v>
       </c>
       <c r="E113" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -10162,7 +10168,7 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J113">
         <v>2.375</v>
@@ -10230,16 +10236,16 @@
         <v>7011606</v>
       </c>
       <c r="C114" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D114" s="2">
         <v>45340.45833333334</v>
       </c>
       <c r="E114" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F114" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G114">
         <v>1</v>
@@ -10248,7 +10254,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J114">
         <v>2.2</v>
@@ -10316,16 +10322,16 @@
         <v>7011610</v>
       </c>
       <c r="C115" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D115" s="2">
         <v>45345.41666666666</v>
       </c>
       <c r="E115" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F115" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G115">
         <v>2</v>
@@ -10334,7 +10340,7 @@
         <v>1</v>
       </c>
       <c r="I115" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J115">
         <v>2</v>
@@ -10402,16 +10408,16 @@
         <v>7011608</v>
       </c>
       <c r="C116" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D116" s="2">
         <v>45346.33333333334</v>
       </c>
       <c r="E116" t="s">
+        <v>39</v>
+      </c>
+      <c r="F116" t="s">
         <v>37</v>
-      </c>
-      <c r="F116" t="s">
-        <v>35</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -10420,7 +10426,7 @@
         <v>1</v>
       </c>
       <c r="I116" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J116">
         <v>3.4</v>
@@ -10488,16 +10494,16 @@
         <v>7011611</v>
       </c>
       <c r="C117" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D117" s="2">
         <v>45346.4375</v>
       </c>
       <c r="E117" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F117" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G117">
         <v>2</v>
@@ -10506,7 +10512,7 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J117">
         <v>2.75</v>
@@ -10574,16 +10580,16 @@
         <v>7011607</v>
       </c>
       <c r="C118" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D118" s="2">
         <v>45347.39583333334</v>
       </c>
       <c r="E118" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F118" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -10592,7 +10598,7 @@
         <v>3</v>
       </c>
       <c r="I118" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J118">
         <v>2.25</v>
@@ -10660,16 +10666,16 @@
         <v>7809824</v>
       </c>
       <c r="C119" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D119" s="2">
         <v>45347.5</v>
       </c>
       <c r="E119" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F119" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G119">
         <v>2</v>
@@ -10678,7 +10684,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J119">
         <v>1.333</v>
@@ -10746,16 +10752,16 @@
         <v>7810273</v>
       </c>
       <c r="C120" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D120" s="2">
         <v>45350.5</v>
       </c>
       <c r="E120" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F120" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -10764,7 +10770,7 @@
         <v>4</v>
       </c>
       <c r="I120" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J120">
         <v>9</v>
@@ -10832,16 +10838,16 @@
         <v>7898044</v>
       </c>
       <c r="C121" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D121" s="2">
         <v>45352.5</v>
       </c>
       <c r="E121" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F121" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G121">
         <v>1</v>
@@ -10850,7 +10856,7 @@
         <v>3</v>
       </c>
       <c r="I121" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J121">
         <v>1.727</v>
@@ -10918,16 +10924,16 @@
         <v>7011616</v>
       </c>
       <c r="C122" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D122" s="2">
         <v>45353.375</v>
       </c>
       <c r="E122" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F122" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G122">
         <v>1</v>
@@ -10936,7 +10942,7 @@
         <v>1</v>
       </c>
       <c r="I122" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J122">
         <v>2.2</v>
@@ -11004,16 +11010,16 @@
         <v>7011612</v>
       </c>
       <c r="C123" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D123" s="2">
         <v>45353.47916666666</v>
       </c>
       <c r="E123" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F123" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G123">
         <v>2</v>
@@ -11022,7 +11028,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J123">
         <v>1.85</v>
@@ -11090,16 +11096,16 @@
         <v>7011613</v>
       </c>
       <c r="C124" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D124" s="2">
         <v>45354.375</v>
       </c>
       <c r="E124" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F124" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G124">
         <v>2</v>
@@ -11108,7 +11114,7 @@
         <v>3</v>
       </c>
       <c r="I124" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J124">
         <v>3.6</v>
@@ -11176,16 +11182,16 @@
         <v>7011615</v>
       </c>
       <c r="C125" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D125" s="2">
         <v>45354.5</v>
       </c>
       <c r="E125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -11194,7 +11200,7 @@
         <v>4</v>
       </c>
       <c r="I125" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J125">
         <v>4.75</v>
@@ -11262,16 +11268,16 @@
         <v>7011620</v>
       </c>
       <c r="C126" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D126" s="2">
         <v>45359.5</v>
       </c>
       <c r="E126" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F126" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -11280,7 +11286,7 @@
         <v>1</v>
       </c>
       <c r="I126" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J126">
         <v>2.2</v>
@@ -11348,16 +11354,16 @@
         <v>7011619</v>
       </c>
       <c r="C127" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D127" s="2">
         <v>45360.33333333334</v>
       </c>
       <c r="E127" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F127" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G127">
         <v>3</v>
@@ -11366,7 +11372,7 @@
         <v>3</v>
       </c>
       <c r="I127" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J127">
         <v>3.5</v>
@@ -11434,16 +11440,16 @@
         <v>7011621</v>
       </c>
       <c r="C128" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D128" s="2">
         <v>45360.4375</v>
       </c>
       <c r="E128" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F128" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G128">
         <v>2</v>
@@ -11452,7 +11458,7 @@
         <v>1</v>
       </c>
       <c r="I128" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J128">
         <v>1.4</v>
@@ -11520,16 +11526,16 @@
         <v>7011617</v>
       </c>
       <c r="C129" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D129" s="2">
         <v>45361.35416666666</v>
       </c>
       <c r="E129" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F129" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G129">
         <v>2</v>
@@ -11538,7 +11544,7 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J129">
         <v>2.3</v>
@@ -11606,16 +11612,16 @@
         <v>7011618</v>
       </c>
       <c r="C130" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D130" s="2">
         <v>45361.45833333334</v>
       </c>
       <c r="E130" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F130" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G130">
         <v>3</v>
@@ -11624,7 +11630,7 @@
         <v>1</v>
       </c>
       <c r="I130" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J130">
         <v>1.4</v>
@@ -11692,16 +11698,16 @@
         <v>7011624</v>
       </c>
       <c r="C131" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D131" s="2">
         <v>45366.5</v>
       </c>
       <c r="E131" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F131" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G131">
         <v>3</v>
@@ -11710,7 +11716,7 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J131">
         <v>2.1</v>
@@ -11778,16 +11784,16 @@
         <v>7011625</v>
       </c>
       <c r="C132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D132" s="2">
         <v>45367.375</v>
       </c>
       <c r="E132" t="s">
+        <v>36</v>
+      </c>
+      <c r="F132" t="s">
         <v>34</v>
-      </c>
-      <c r="F132" t="s">
-        <v>32</v>
       </c>
       <c r="G132">
         <v>2</v>
@@ -11796,7 +11802,7 @@
         <v>1</v>
       </c>
       <c r="I132" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J132">
         <v>1.85</v>
@@ -11864,16 +11870,16 @@
         <v>7011622</v>
       </c>
       <c r="C133" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D133" s="2">
         <v>45367.47916666666</v>
       </c>
       <c r="E133" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F133" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -11882,7 +11888,7 @@
         <v>1</v>
       </c>
       <c r="I133" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J133">
         <v>1.85</v>
@@ -11950,16 +11956,16 @@
         <v>7011626</v>
       </c>
       <c r="C134" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D134" s="2">
         <v>45368.375</v>
       </c>
       <c r="E134" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F134" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G134">
         <v>1</v>
@@ -11968,7 +11974,7 @@
         <v>3</v>
       </c>
       <c r="I134" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J134">
         <v>4.333</v>
@@ -12036,16 +12042,16 @@
         <v>7011623</v>
       </c>
       <c r="C135" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D135" s="2">
         <v>45368.5</v>
       </c>
       <c r="E135" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F135" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G135">
         <v>1</v>
@@ -12054,7 +12060,7 @@
         <v>2</v>
       </c>
       <c r="I135" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J135">
         <v>2.9</v>
@@ -12122,16 +12128,16 @@
         <v>7011628</v>
       </c>
       <c r="C136" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D136" s="2">
         <v>45380.39583333334</v>
       </c>
       <c r="E136" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F136" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G136">
         <v>0</v>
@@ -12140,7 +12146,7 @@
         <v>1</v>
       </c>
       <c r="I136" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J136">
         <v>3.5</v>
@@ -12208,16 +12214,16 @@
         <v>7011631</v>
       </c>
       <c r="C137" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D137" s="2">
         <v>45380.5</v>
       </c>
       <c r="E137" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F137" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G137">
         <v>1</v>
@@ -12226,7 +12232,7 @@
         <v>6</v>
       </c>
       <c r="I137" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J137">
         <v>6</v>
@@ -12294,16 +12300,16 @@
         <v>7011630</v>
       </c>
       <c r="C138" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D138" s="2">
         <v>45381.39583333334</v>
       </c>
       <c r="E138" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F138" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -12312,7 +12318,7 @@
         <v>1</v>
       </c>
       <c r="I138" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J138">
         <v>2.3</v>
@@ -12380,16 +12386,16 @@
         <v>7011629</v>
       </c>
       <c r="C139" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D139" s="2">
         <v>45381.5</v>
       </c>
       <c r="E139" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F139" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -12398,7 +12404,7 @@
         <v>1</v>
       </c>
       <c r="I139" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J139">
         <v>2.1</v>
@@ -12466,16 +12472,16 @@
         <v>7011627</v>
       </c>
       <c r="C140" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D140" s="2">
         <v>45382.45833333334</v>
       </c>
       <c r="E140" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F140" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -12484,7 +12490,7 @@
         <v>0</v>
       </c>
       <c r="I140" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J140">
         <v>1.95</v>
@@ -12552,16 +12558,16 @@
         <v>7011632</v>
       </c>
       <c r="C141" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D141" s="2">
         <v>45387.54166666666</v>
       </c>
       <c r="E141" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F141" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -12570,7 +12576,7 @@
         <v>2</v>
       </c>
       <c r="I141" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J141">
         <v>2.1</v>
@@ -12638,16 +12644,16 @@
         <v>7011634</v>
       </c>
       <c r="C142" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D142" s="2">
         <v>45388.375</v>
       </c>
       <c r="E142" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F142" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G142">
         <v>2</v>
@@ -12656,7 +12662,7 @@
         <v>0</v>
       </c>
       <c r="I142" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J142">
         <v>2.55</v>
@@ -12724,16 +12730,16 @@
         <v>7011633</v>
       </c>
       <c r="C143" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D143" s="2">
         <v>45388.54166666666</v>
       </c>
       <c r="E143" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F143" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G143">
         <v>4</v>
@@ -12742,7 +12748,7 @@
         <v>2</v>
       </c>
       <c r="I143" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J143">
         <v>1.222</v>
@@ -12810,16 +12816,16 @@
         <v>7011635</v>
       </c>
       <c r="C144" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D144" s="2">
         <v>45389.39583333334</v>
       </c>
       <c r="E144" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F144" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G144">
         <v>4</v>
@@ -12828,7 +12834,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J144">
         <v>1.4</v>
@@ -12896,16 +12902,16 @@
         <v>7011636</v>
       </c>
       <c r="C145" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D145" s="2">
         <v>45389.54166666666</v>
       </c>
       <c r="E145" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F145" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G145">
         <v>1</v>
@@ -12914,7 +12920,7 @@
         <v>1</v>
       </c>
       <c r="I145" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J145">
         <v>1.727</v>
@@ -12982,16 +12988,16 @@
         <v>7011638</v>
       </c>
       <c r="C146" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D146" s="2">
         <v>45394.5</v>
       </c>
       <c r="E146" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F146" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G146">
         <v>0</v>
@@ -13000,7 +13006,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J146">
         <v>2.9</v>
@@ -13068,16 +13074,16 @@
         <v>7011639</v>
       </c>
       <c r="C147" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D147" s="2">
         <v>45395.39583333334</v>
       </c>
       <c r="E147" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F147" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G147">
         <v>1</v>
@@ -13086,7 +13092,7 @@
         <v>2</v>
       </c>
       <c r="I147" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J147">
         <v>3</v>
@@ -13154,16 +13160,16 @@
         <v>7011637</v>
       </c>
       <c r="C148" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D148" s="2">
         <v>45395.5</v>
       </c>
       <c r="E148" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F148" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G148">
         <v>3</v>
@@ -13172,7 +13178,7 @@
         <v>0</v>
       </c>
       <c r="I148" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J148">
         <v>1.833</v>
@@ -13240,16 +13246,16 @@
         <v>7011640</v>
       </c>
       <c r="C149" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D149" s="2">
         <v>45396.39583333334</v>
       </c>
       <c r="E149" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F149" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G149">
         <v>3</v>
@@ -13258,7 +13264,7 @@
         <v>3</v>
       </c>
       <c r="I149" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J149">
         <v>1.727</v>
@@ -13326,16 +13332,16 @@
         <v>7012356</v>
       </c>
       <c r="C150" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D150" s="2">
         <v>45396.5</v>
       </c>
       <c r="E150" t="s">
+        <v>35</v>
+      </c>
+      <c r="F150" t="s">
         <v>33</v>
-      </c>
-      <c r="F150" t="s">
-        <v>31</v>
       </c>
       <c r="G150">
         <v>3</v>
@@ -13344,7 +13350,7 @@
         <v>2</v>
       </c>
       <c r="I150" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J150">
         <v>2.625</v>
@@ -13412,16 +13418,16 @@
         <v>7020807</v>
       </c>
       <c r="C151" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D151" s="2">
         <v>45401.39583333334</v>
       </c>
       <c r="E151" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F151" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G151">
         <v>1</v>
@@ -13430,7 +13436,7 @@
         <v>4</v>
       </c>
       <c r="I151" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J151">
         <v>2.25</v>
@@ -13498,16 +13504,16 @@
         <v>7029131</v>
       </c>
       <c r="C152" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D152" s="2">
         <v>45402.39583333334</v>
       </c>
       <c r="E152" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F152" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G152">
         <v>2</v>
@@ -13516,7 +13522,7 @@
         <v>2</v>
       </c>
       <c r="I152" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J152">
         <v>1.166</v>
@@ -13584,16 +13590,16 @@
         <v>7025505</v>
       </c>
       <c r="C153" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D153" s="2">
         <v>45402.5</v>
       </c>
       <c r="E153" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F153" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G153">
         <v>3</v>
@@ -13602,7 +13608,7 @@
         <v>1</v>
       </c>
       <c r="I153" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J153">
         <v>2.1</v>
@@ -13670,16 +13676,16 @@
         <v>7027687</v>
       </c>
       <c r="C154" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D154" s="2">
         <v>45403.39583333334</v>
       </c>
       <c r="E154" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F154" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G154">
         <v>1</v>
@@ -13688,7 +13694,7 @@
         <v>2</v>
       </c>
       <c r="I154" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J154">
         <v>2.75</v>
@@ -13756,16 +13762,16 @@
         <v>7020806</v>
       </c>
       <c r="C155" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D155" s="2">
         <v>45403.5</v>
       </c>
       <c r="E155" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F155" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G155">
         <v>0</v>
@@ -13774,7 +13780,7 @@
         <v>2</v>
       </c>
       <c r="I155" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J155">
         <v>2.5</v>
@@ -13842,60 +13848,190 @@
         <v>27</v>
       </c>
       <c r="C156" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D156" s="2">
-        <v>45409.45833333334</v>
+        <v>45410.44791666666</v>
       </c>
       <c r="E156" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F156" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J156">
-        <v>1.85</v>
+        <v>2.25</v>
       </c>
       <c r="K156">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="L156">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="M156">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="N156">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="O156">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P156">
         <v>-0.5</v>
       </c>
       <c r="Q156">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R156">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S156">
         <v>2.5</v>
       </c>
       <c r="T156">
+        <v>1.95</v>
+      </c>
+      <c r="U156">
         <v>1.85</v>
       </c>
-      <c r="U156">
+      <c r="V156">
+        <v>0</v>
+      </c>
+      <c r="W156">
+        <v>0</v>
+      </c>
+      <c r="X156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:28">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157" t="s">
+        <v>28</v>
+      </c>
+      <c r="C157" t="s">
+        <v>30</v>
+      </c>
+      <c r="D157" s="2">
+        <v>45410.54166666666</v>
+      </c>
+      <c r="E157" t="s">
+        <v>40</v>
+      </c>
+      <c r="F157" t="s">
+        <v>33</v>
+      </c>
+      <c r="J157">
+        <v>4.75</v>
+      </c>
+      <c r="K157">
+        <v>4.2</v>
+      </c>
+      <c r="L157">
+        <v>1.5</v>
+      </c>
+      <c r="M157">
+        <v>4.75</v>
+      </c>
+      <c r="N157">
+        <v>4.2</v>
+      </c>
+      <c r="O157">
+        <v>1.5</v>
+      </c>
+      <c r="P157">
+        <v>1</v>
+      </c>
+      <c r="Q157">
         <v>1.95</v>
       </c>
-      <c r="V156">
-        <v>0</v>
-      </c>
-      <c r="W156">
-        <v>0</v>
-      </c>
-      <c r="X156">
+      <c r="R157">
+        <v>1.85</v>
+      </c>
+      <c r="S157">
+        <v>3</v>
+      </c>
+      <c r="T157">
+        <v>2</v>
+      </c>
+      <c r="U157">
+        <v>1.8</v>
+      </c>
+      <c r="V157">
+        <v>0</v>
+      </c>
+      <c r="W157">
+        <v>0</v>
+      </c>
+      <c r="X157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:28">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158" t="s">
+        <v>29</v>
+      </c>
+      <c r="C158" t="s">
+        <v>30</v>
+      </c>
+      <c r="D158" s="2">
+        <v>45411.5</v>
+      </c>
+      <c r="E158" t="s">
+        <v>36</v>
+      </c>
+      <c r="F158" t="s">
+        <v>31</v>
+      </c>
+      <c r="J158">
+        <v>1.571</v>
+      </c>
+      <c r="K158">
+        <v>4</v>
+      </c>
+      <c r="L158">
+        <v>4.333</v>
+      </c>
+      <c r="M158">
+        <v>1.45</v>
+      </c>
+      <c r="N158">
+        <v>4.2</v>
+      </c>
+      <c r="O158">
+        <v>5.25</v>
+      </c>
+      <c r="P158">
+        <v>-1</v>
+      </c>
+      <c r="Q158">
+        <v>1.775</v>
+      </c>
+      <c r="R158">
+        <v>2.025</v>
+      </c>
+      <c r="S158">
+        <v>2.25</v>
+      </c>
+      <c r="T158">
+        <v>1.9</v>
+      </c>
+      <c r="U158">
+        <v>1.9</v>
+      </c>
+      <c r="V158">
+        <v>0</v>
+      </c>
+      <c r="W158">
+        <v>0</v>
+      </c>
+      <c r="X158">
         <v>0</v>
       </c>
     </row>

</xml_diff>